<commit_message>
File organising. MTFLOW is now validated w.r.t. X22A data
</commit_message>
<xml_diff>
--- a/Validation/WindTunnelData.xlsx
+++ b/Validation/WindTunnelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/B266C95A83FBF4BB/Documenten/TU Delft Aerospace Engineering/Msc2/AE5222 - Thesis/Software/Conceptual-Investigation-of-Alternative-Electric-Ducted-Fan-Architectures/Validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="755" documentId="8_{E7BF6703-466F-4498-AEEA-FFB8403C4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B92D9F8D-569C-400E-A5C0-F777EBF6D525}"/>
+  <xr:revisionPtr revIDLastSave="820" documentId="8_{E7BF6703-466F-4498-AEEA-FFB8403C4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{332B901C-7DFC-44FC-A966-C703AC4F77AC}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="2" xr2:uid="{6111FCF9-37F3-4199-9E4E-EEB7F0803D9A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="2" xr2:uid="{6111FCF9-37F3-4199-9E4E-EEB7F0803D9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Wind Tunnel Beta=29deg data" sheetId="16" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t>CT</t>
   </si>
@@ -150,12 +150,18 @@
   <si>
     <t>Inviscid analysis only</t>
   </si>
+  <si>
+    <t>Ctuncertainty</t>
+  </si>
+  <si>
+    <t>Cpuncertainty</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,12 +184,6 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -229,16 +229,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="14">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1426,7 +1438,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="en-GB"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1440,13 +1452,11 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>MTFLOW Beta=29deg</c:v>
+            <c:v>MTFLOW</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1531,24 +1541,20 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>CT Wind Tunnel Beta=29deg</c:v>
+            <c:v>Wind Tunnel</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="star"/>
             <c:size val="5"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
@@ -1580,9 +1586,68 @@
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
-            <c:errValType val="fixedVal"/>
+            <c:errValType val="cust"/>
             <c:noEndCap val="0"/>
-            <c:val val="1.0000000000000002E-2"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Wind Tunnel Beta=29deg data'!$K$6:$K$12</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0.22222222222222224</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.16326530612244899</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.12499999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.8765432098765427E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.08</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6.6115702479338831E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.5555555555555559E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Wind Tunnel Beta=29deg data'!$K$6:$K$12</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0.22222222222222224</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.16326530612244899</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.12499999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.8765432098765427E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.08</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6.6115702479338831E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.5555555555555559E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
             <c:spPr>
               <a:noFill/>
               <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1696,6 +1761,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1814,6 +1893,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2066,7 +2159,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="LID4096"/>
+          <a:endParaRPr lang="en-GB"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2080,13 +2173,11 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>CT Wind Tunnel Beta=19deg</c:v>
+            <c:v>Wind Tunnel</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2106,6 +2197,105 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Wind Tunnel Beta=19deg data'!$K$6:$K$12</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0.22222222222222224</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.16326530612244899</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.12499999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.8765432098765427E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.08</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6.6115702479338831E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.5555555555555559E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Wind Tunnel Beta=19deg data'!$K$6:$K$12</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0.22222222222222224</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.16326530612244899</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.12499999999999997</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>9.8765432098765427E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.08</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6.6115702479338831E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.5555555555555559E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1.0000000000000002E-2"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>'Wind Tunnel Beta=19deg data'!$G$6:$G$12</c:f>
@@ -2177,19 +2367,17 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>MTFLOW Beta=19deg</c:v>
+            <c:v>MTFLOW</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
+            <c:symbol val="triangle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -2299,6 +2487,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2422,6 +2624,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -2520,6 +2736,1536 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="1167254607"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Comparison for </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="el-GR" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>β</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>=29</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Grotesque" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>˚</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MTFLOW</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'test results'!$I$3:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'test results'!$K$3:$K$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="2">
+                  <c:v>5.8262999999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1558999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3298000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7305999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-13BD-4DDA-8799-69A4B5EA0FC9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Wind Tunnel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1.0000000000000002E-2"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Wind Tunnel Beta=29deg data'!$L$6:$L$12</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0.74074074074074081</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.46647230320699723</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.31249999999999994</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.21947873799725648</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.16</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.12021036814425241</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>9.2592592592592601E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Wind Tunnel Beta=29deg data'!$L$6:$L$12</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0.74074074074074081</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.46647230320699723</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.31249999999999994</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.21947873799725648</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.16</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.12021036814425241</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>9.2592592592592601E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wind Tunnel Beta=29deg data'!$G$6:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wind Tunnel Beta=29deg data'!$I$6:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>17.866666666666667</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.032069970845484</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.159374999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.8658436213991765</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4304000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4522915101427487</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7824074074074074</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-13BD-4DDA-8799-69A4B5EA0FC9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="923558143"/>
+        <c:axId val="923554783"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="923558143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Advance Ratio J [-]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="923554783"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="923554783"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Power</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Coefficient CP </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>[-]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="923558143"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Comparison for </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="el-GR" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>β</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>=19</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Grotesque" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>˚</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MTFLOW</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'test results'!$I$13:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'test results'!$K$13:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="1">
+                  <c:v>3.5183</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1171000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3049999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.80198999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.49051</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.29032000000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3F79-4D15-A321-F6B85F64626E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Wind Tunnel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1.0000000000000002E-2"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Wind Tunnel Beta=19deg data'!$L$6:$L$12</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0.74074074074074081</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.46647230320699723</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.31249999999999994</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.21947873799725648</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.16</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.12021036814425241</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>9.2592592592592601E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Wind Tunnel Beta=19deg data'!$L$6:$L$12</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0.74074074074074081</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.46647230320699723</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.31249999999999994</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.21947873799725648</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.16</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.12021036814425241</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>9.2592592592592601E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wind Tunnel Beta=19deg data'!$G$6:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wind Tunnel Beta=19deg data'!$I$6:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.9511111111111115</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.2075801749271147</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6699999999999995</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7380521262002742</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1491199999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.77499624342599527</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.53888888888888886</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3F79-4D15-A321-F6B85F64626E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="923558143"/>
+        <c:axId val="923554783"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="923558143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Advance Ratio J [-]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="923554783"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="923554783"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Power</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> Coefficient CP </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>[-]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="923558143"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2799,6 +4545,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -4864,6 +6690,1038 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5506,15 +8364,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>288925</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:colOff>332740</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>8255</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>593725</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>60325</xdr:rowOff>
+      <xdr:colOff>637540</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161290</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5544,15 +8402,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>314960</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>170236</xdr:rowOff>
+      <xdr:colOff>313079</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>171027</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>404578</xdr:colOff>
+      <xdr:colOff>630877</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>115141</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5579,6 +8437,82 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>638794</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>300347</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>162560</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C98D548-8505-4177-B61B-3C05C33DF76F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>627066</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>172241</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>296883</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>134009</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E57ABB2-42AB-4F02-BE41-381EB9561BA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5595,7 +8529,7 @@
     <tableColumn id="1" xr3:uid="{29ABFF0D-E0B2-47B7-91D1-13ECB5D2F91C}" name="J"/>
     <tableColumn id="2" xr3:uid="{D1C4D961-3359-484B-AC98-CD0007496AF4}" name="C_T"/>
     <tableColumn id="3" xr3:uid="{4AFBF296-9077-4A54-9E31-6E461321828F}" name="C_P"/>
-    <tableColumn id="4" xr3:uid="{A0AE88A3-F978-48D2-BECE-0446AF96AAAB}" name="Eta" dataDxfId="0">
+    <tableColumn id="4" xr3:uid="{A0AE88A3-F978-48D2-BECE-0446AF96AAAB}" name="Eta" dataDxfId="13">
       <calculatedColumnFormula>Table1[[#This Row],[C_T]]/Table1[[#This Row],[C_P]]*Table1[[#This Row],[J]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5604,20 +8538,26 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{89469267-DFAB-445F-A105-A03D872ECC3C}" name="Table2" displayName="Table2" ref="G5:J12" totalsRowShown="0">
-  <autoFilter ref="G5:J12" xr:uid="{89469267-DFAB-445F-A105-A03D872ECC3C}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E3D689F5-B43D-4B53-B3BC-A1930A9A680A}" name="J" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{89469267-DFAB-445F-A105-A03D872ECC3C}" name="Table2" displayName="Table2" ref="G5:L12" totalsRowShown="0">
+  <autoFilter ref="G5:L12" xr:uid="{89469267-DFAB-445F-A105-A03D872ECC3C}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{E3D689F5-B43D-4B53-B3BC-A1930A9A680A}" name="J" dataDxfId="12">
       <calculatedColumnFormula>Table1[[#This Row],[J]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{A90F5A15-4E8F-42CD-B615-C0FA79DD1536}" name="C_T" dataDxfId="8">
+    <tableColumn id="2" xr3:uid="{A90F5A15-4E8F-42CD-B615-C0FA79DD1536}" name="C_T" dataDxfId="11">
       <calculatedColumnFormula>Table1[[#This Row],[C_T]]*2/POWER(Table1[[#This Row],[J]],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A0A7E7C4-CFC3-4CA8-9478-AFCD0D800B2B}" name="C_P" dataDxfId="4">
+    <tableColumn id="3" xr3:uid="{A0A7E7C4-CFC3-4CA8-9478-AFCD0D800B2B}" name="C_P" dataDxfId="10">
       <calculatedColumnFormula>Table1[[#This Row],[C_P]]*2/POWER(Table2[[#This Row],[J]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{18B4E670-68E4-4D17-B399-7D20B93C204F}" name="Eta" dataDxfId="1">
+    <tableColumn id="4" xr3:uid="{18B4E670-68E4-4D17-B399-7D20B93C204F}" name="Eta" dataDxfId="9">
       <calculatedColumnFormula>Table2[[#This Row],[C_T]]/Table2[[#This Row],[C_P]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{4C8B0383-C909-4D83-9235-2400B5825E21}" name="Ctuncertainty" dataDxfId="3">
+      <calculatedColumnFormula>0.01*2/POWER(Table2[[#This Row],[J]],2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{10742F03-23FF-483A-AAFB-71F114837A71}" name="Cpuncertainty" dataDxfId="2">
+      <calculatedColumnFormula>0.01*2/POWER(Table2[[#This Row],[J]],3)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5631,7 +8571,7 @@
     <tableColumn id="1" xr3:uid="{C149BBF6-A8E9-4EBB-9499-1359884248B9}" name="J"/>
     <tableColumn id="2" xr3:uid="{944C6200-702E-4286-A1C4-A0B13B1C2582}" name="C_T"/>
     <tableColumn id="3" xr3:uid="{0C234C63-EAC7-4DA5-A621-F79654C1515D}" name="C_P"/>
-    <tableColumn id="4" xr3:uid="{85015DF5-982B-45C5-8783-398164E6F3D2}" name="Eta" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{85015DF5-982B-45C5-8783-398164E6F3D2}" name="Eta" dataDxfId="8">
       <calculatedColumnFormula>Table14[[#This Row],[C_T]]/Table14[[#This Row],[C_P]]*Table14[[#This Row],[J]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5640,9 +8580,9 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9B8DCF99-C126-46A4-BEB0-1ACA0793BD79}" name="Table25" displayName="Table25" ref="G5:J12" totalsRowShown="0">
-  <autoFilter ref="G5:J12" xr:uid="{89469267-DFAB-445F-A105-A03D872ECC3C}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9B8DCF99-C126-46A4-BEB0-1ACA0793BD79}" name="Table25" displayName="Table25" ref="G5:L12" totalsRowShown="0">
+  <autoFilter ref="G5:L12" xr:uid="{89469267-DFAB-445F-A105-A03D872ECC3C}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{85258774-B764-4008-955C-0BE292368B91}" name="J" dataDxfId="7">
       <calculatedColumnFormula>Table14[[#This Row],[J]]</calculatedColumnFormula>
     </tableColumn>
@@ -5652,8 +8592,14 @@
     <tableColumn id="3" xr3:uid="{9C4FE48A-1F92-49E4-97E7-D97D0A26F74A}" name="C_P" dataDxfId="5">
       <calculatedColumnFormula>Table14[[#This Row],[C_P]]*2/POWER(Table25[[#This Row],[J]],3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EF4FF774-63A0-405E-A48F-EC42A8ECE784}" name="Eta" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{EF4FF774-63A0-405E-A48F-EC42A8ECE784}" name="Eta" dataDxfId="4">
       <calculatedColumnFormula>Table25[[#This Row],[C_T]]/Table25[[#This Row],[C_P]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{E32AD299-DD16-411F-888C-B7774AE0432F}" name="Ctuncertainty" dataDxfId="1">
+      <calculatedColumnFormula>0.01*2/POWER(Table2[[#This Row],[J]],2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{7EE5D3F7-E013-4DDF-A5A6-7A6A7B15A183}" name="Cpuncertainty" dataDxfId="0">
+      <calculatedColumnFormula>0.01*2/POWER(Table2[[#This Row],[J]],3)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5991,30 +8937,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B26E69B-6441-4D2A-91E2-CF3588D774EF}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5:L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -6022,7 +8968,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -6047,8 +8993,14 @@
       <c r="J5" t="s">
         <v>17</v>
       </c>
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>0.3</v>
       </c>
@@ -6074,12 +9026,20 @@
         <f>Table1[[#This Row],[C_P]]*2/POWER(Table2[[#This Row],[J]],3)</f>
         <v>17.866666666666667</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6">
         <f>Table2[[#This Row],[C_T]]/Table2[[#This Row],[C_P]]</f>
         <v>0.4648009950248756</v>
       </c>
+      <c r="K6" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>0.22222222222222224</v>
+      </c>
+      <c r="L6" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>0.74074074074074081</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>0.35</v>
       </c>
@@ -6093,11 +9053,11 @@
         <f>Table1[[#This Row],[C_T]]/Table1[[#This Row],[C_P]]*Table1[[#This Row],[J]]</f>
         <v>0.51797040169133191</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7">
         <f>Table1[[#This Row],[J]]</f>
         <v>0.35</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7">
         <f>Table1[[#This Row],[C_T]]*2/POWER(Table1[[#This Row],[J]],2)</f>
         <v>5.7142857142857144</v>
       </c>
@@ -6105,12 +9065,20 @@
         <f>Table1[[#This Row],[C_P]]*2/POWER(Table2[[#This Row],[J]],3)</f>
         <v>11.032069970845484</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7">
         <f>Table2[[#This Row],[C_T]]/Table2[[#This Row],[C_P]]</f>
         <v>0.51797040169133179</v>
       </c>
+      <c r="K7" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>0.16326530612244899</v>
+      </c>
+      <c r="L7" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>0.46647230320699723</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>0.4</v>
       </c>
@@ -6124,11 +9092,11 @@
         <f>Table1[[#This Row],[C_T]]/Table1[[#This Row],[C_P]]*Table1[[#This Row],[J]]</f>
         <v>0.5587079877782628</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8">
         <f>Table1[[#This Row],[J]]</f>
         <v>0.4</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8">
         <f>Table1[[#This Row],[C_T]]*2/POWER(Table1[[#This Row],[J]],2)</f>
         <v>3.9999999999999991</v>
       </c>
@@ -6136,12 +9104,20 @@
         <f>Table1[[#This Row],[C_P]]*2/POWER(Table2[[#This Row],[J]],3)</f>
         <v>7.159374999999998</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8">
         <f>Table2[[#This Row],[C_T]]/Table2[[#This Row],[C_P]]</f>
         <v>0.5587079877782628</v>
       </c>
+      <c r="K8" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>0.12499999999999997</v>
+      </c>
+      <c r="L8" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>0.31249999999999994</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>0.45</v>
       </c>
@@ -6155,11 +9131,11 @@
         <f>Table1[[#This Row],[C_T]]/Table1[[#This Row],[C_P]]*Table1[[#This Row],[J]]</f>
         <v>0.60081190798376183</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9">
         <f>Table1[[#This Row],[J]]</f>
         <v>0.45</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9">
         <f>Table1[[#This Row],[C_T]]*2/POWER(Table1[[#This Row],[J]],2)</f>
         <v>2.9234567901234563</v>
       </c>
@@ -6167,12 +9143,20 @@
         <f>Table1[[#This Row],[C_P]]*2/POWER(Table2[[#This Row],[J]],3)</f>
         <v>4.8658436213991765</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9">
         <f>Table2[[#This Row],[C_T]]/Table2[[#This Row],[C_P]]</f>
         <v>0.60081190798376183</v>
       </c>
+      <c r="K9" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>9.8765432098765427E-2</v>
+      </c>
+      <c r="L9" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>0.21947873799725648</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>0.5</v>
       </c>
@@ -6186,11 +9170,11 @@
         <f>Table1[[#This Row],[C_T]]/Table1[[#This Row],[C_P]]*Table1[[#This Row],[J]]</f>
         <v>0.62966417910447758</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10">
         <f>Table1[[#This Row],[J]]</f>
         <v>0.5</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10">
         <f>Table1[[#This Row],[C_T]]*2/POWER(Table1[[#This Row],[J]],2)</f>
         <v>2.16</v>
       </c>
@@ -6198,12 +9182,20 @@
         <f>Table1[[#This Row],[C_P]]*2/POWER(Table2[[#This Row],[J]],3)</f>
         <v>3.4304000000000001</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10">
         <f>Table2[[#This Row],[C_T]]/Table2[[#This Row],[C_P]]</f>
         <v>0.62966417910447758</v>
       </c>
+      <c r="K10" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>0.08</v>
+      </c>
+      <c r="L10" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>0.16</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>0.55000000000000004</v>
       </c>
@@ -6217,11 +9209,11 @@
         <f>Table1[[#This Row],[C_T]]/Table1[[#This Row],[C_P]]*Table1[[#This Row],[J]]</f>
         <v>0.66323529411764715</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11">
         <f>Table1[[#This Row],[J]]</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11">
         <f>Table1[[#This Row],[C_T]]*2/POWER(Table1[[#This Row],[J]],2)</f>
         <v>1.6264462809917353</v>
       </c>
@@ -6229,12 +9221,20 @@
         <f>Table1[[#This Row],[C_P]]*2/POWER(Table2[[#This Row],[J]],3)</f>
         <v>2.4522915101427487</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11">
         <f>Table2[[#This Row],[C_T]]/Table2[[#This Row],[C_P]]</f>
         <v>0.66323529411764726</v>
       </c>
+      <c r="K11" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>6.6115702479338831E-2</v>
+      </c>
+      <c r="L11" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>0.12021036814425241</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>0.6</v>
       </c>
@@ -6248,11 +9248,11 @@
         <f>Table1[[#This Row],[C_T]]/Table1[[#This Row],[C_P]]*Table1[[#This Row],[J]]</f>
         <v>0.68571428571428561</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12">
         <f>Table1[[#This Row],[J]]</f>
         <v>0.6</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12">
         <f>Table1[[#This Row],[C_T]]*2/POWER(Table1[[#This Row],[J]],2)</f>
         <v>1.2222222222222223</v>
       </c>
@@ -6260,9 +9260,17 @@
         <f>Table1[[#This Row],[C_P]]*2/POWER(Table2[[#This Row],[J]],3)</f>
         <v>1.7824074074074074</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12">
         <f>Table2[[#This Row],[C_T]]/Table2[[#This Row],[C_P]]</f>
         <v>0.68571428571428572</v>
+      </c>
+      <c r="K12" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>5.5555555555555559E-2</v>
+      </c>
+      <c r="L12" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>9.2592592592592601E-2</v>
       </c>
     </row>
   </sheetData>
@@ -6281,30 +9289,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CBD950F-5FB4-419F-B6AE-C3E6C12B06BE}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -6312,7 +9320,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -6337,8 +9345,14 @@
       <c r="J5" t="s">
         <v>17</v>
       </c>
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>0.3</v>
       </c>
@@ -6364,12 +9378,20 @@
         <f>Table14[[#This Row],[C_P]]*2/POWER(Table25[[#This Row],[J]],3)</f>
         <v>6.9511111111111115</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6">
         <f>Table25[[#This Row],[C_T]]/Table25[[#This Row],[C_P]]</f>
         <v>0.54187979539641951</v>
       </c>
+      <c r="K6" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>0.22222222222222224</v>
+      </c>
+      <c r="L6" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>0.74074074074074081</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>0.35</v>
       </c>
@@ -6383,11 +9405,11 @@
         <f>Table14[[#This Row],[C_T]]/Table14[[#This Row],[C_P]]*Table14[[#This Row],[J]]</f>
         <v>0.58009977827050985</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7">
         <f>Table14[[#This Row],[J]]</f>
         <v>0.35</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7">
         <f>Table14[[#This Row],[C_T]]*2/POWER(Table14[[#This Row],[J]],2)</f>
         <v>2.4408163265306126</v>
       </c>
@@ -6395,12 +9417,20 @@
         <f>Table14[[#This Row],[C_P]]*2/POWER(Table25[[#This Row],[J]],3)</f>
         <v>4.2075801749271147</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7">
         <f>Table25[[#This Row],[C_T]]/Table25[[#This Row],[C_P]]</f>
         <v>0.58009977827050996</v>
       </c>
+      <c r="K7" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>0.16326530612244899</v>
+      </c>
+      <c r="L7" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>0.46647230320699723</v>
+      </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>0.4</v>
       </c>
@@ -6414,11 +9444,11 @@
         <f>Table14[[#This Row],[C_T]]/Table14[[#This Row],[C_P]]*Table14[[#This Row],[J]]</f>
         <v>0.61189138576779034</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8">
         <f>Table14[[#This Row],[J]]</f>
         <v>0.4</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8">
         <f>Table14[[#This Row],[C_T]]*2/POWER(Table14[[#This Row],[J]],2)</f>
         <v>1.6337499999999998</v>
       </c>
@@ -6426,12 +9456,20 @@
         <f>Table14[[#This Row],[C_P]]*2/POWER(Table25[[#This Row],[J]],3)</f>
         <v>2.6699999999999995</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8">
         <f>Table25[[#This Row],[C_T]]/Table25[[#This Row],[C_P]]</f>
         <v>0.61189138576779034</v>
       </c>
+      <c r="K8" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>0.12499999999999997</v>
+      </c>
+      <c r="L8" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>0.31249999999999994</v>
+      </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>0.45</v>
       </c>
@@ -6445,11 +9483,11 @@
         <f>Table14[[#This Row],[C_T]]/Table14[[#This Row],[C_P]]*Table14[[#This Row],[J]]</f>
         <v>0.6358757418866019</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9">
         <f>Table14[[#This Row],[J]]</f>
         <v>0.45</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9">
         <f>Table14[[#This Row],[C_T]]*2/POWER(Table14[[#This Row],[J]],2)</f>
         <v>1.105185185185185</v>
       </c>
@@ -6457,12 +9495,20 @@
         <f>Table14[[#This Row],[C_P]]*2/POWER(Table25[[#This Row],[J]],3)</f>
         <v>1.7380521262002742</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9">
         <f>Table25[[#This Row],[C_T]]/Table25[[#This Row],[C_P]]</f>
         <v>0.63587574188660179</v>
       </c>
+      <c r="K9" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>9.8765432098765427E-2</v>
+      </c>
+      <c r="L9" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>0.21947873799725648</v>
+      </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>0.5</v>
       </c>
@@ -6476,11 +9522,11 @@
         <f>Table14[[#This Row],[C_T]]/Table14[[#This Row],[C_P]]*Table14[[#This Row],[J]]</f>
         <v>0.62204121414647739</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10">
         <f>Table14[[#This Row],[J]]</f>
         <v>0.5</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10">
         <f>Table14[[#This Row],[C_T]]*2/POWER(Table14[[#This Row],[J]],2)</f>
         <v>0.71479999999999999</v>
       </c>
@@ -6488,12 +9534,20 @@
         <f>Table14[[#This Row],[C_P]]*2/POWER(Table25[[#This Row],[J]],3)</f>
         <v>1.1491199999999999</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10">
         <f>Table25[[#This Row],[C_T]]/Table25[[#This Row],[C_P]]</f>
         <v>0.62204121414647739</v>
       </c>
+      <c r="K10" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>0.08</v>
+      </c>
+      <c r="L10" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>0.16</v>
+      </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>0.55000000000000004</v>
       </c>
@@ -6507,11 +9561,11 @@
         <f>Table14[[#This Row],[C_T]]/Table14[[#This Row],[C_P]]*Table14[[#This Row],[J]]</f>
         <v>0.61270358306188921</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11">
         <f>Table14[[#This Row],[J]]</f>
         <v>0.55000000000000004</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11">
         <f>Table14[[#This Row],[C_T]]*2/POWER(Table14[[#This Row],[J]],2)</f>
         <v>0.47484297520661145</v>
       </c>
@@ -6519,12 +9573,20 @@
         <f>Table14[[#This Row],[C_P]]*2/POWER(Table25[[#This Row],[J]],3)</f>
         <v>0.77499624342599527</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11">
         <f>Table25[[#This Row],[C_T]]/Table25[[#This Row],[C_P]]</f>
         <v>0.61270358306188932</v>
       </c>
+      <c r="K11" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>6.6115702479338831E-2</v>
+      </c>
+      <c r="L11" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>0.12021036814425241</v>
+      </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>0.6</v>
       </c>
@@ -6538,11 +9600,11 @@
         <f>Table14[[#This Row],[C_T]]/Table14[[#This Row],[C_P]]*Table14[[#This Row],[J]]</f>
         <v>0.51546391752577325</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12">
         <f>Table14[[#This Row],[J]]</f>
         <v>0.6</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12">
         <f>Table14[[#This Row],[C_T]]*2/POWER(Table14[[#This Row],[J]],2)</f>
         <v>0.27777777777777779</v>
       </c>
@@ -6550,9 +9612,17 @@
         <f>Table14[[#This Row],[C_P]]*2/POWER(Table25[[#This Row],[J]],3)</f>
         <v>0.53888888888888886</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12">
         <f>Table25[[#This Row],[C_T]]/Table25[[#This Row],[C_P]]</f>
         <v>0.51546391752577325</v>
+      </c>
+      <c r="K12" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],2)</f>
+        <v>5.5555555555555559E-2</v>
+      </c>
+      <c r="L12" s="6">
+        <f>0.01*2/POWER(Table2[[#This Row],[J]],3)</f>
+        <v>9.2592592592592601E-2</v>
       </c>
     </row>
   </sheetData>
@@ -6573,13 +9643,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D17483C-FDF0-45AC-9867-0493571C96AF}">
   <dimension ref="F1:Z19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView tabSelected="1" topLeftCell="H5" zoomScale="77" zoomScaleNormal="97" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="15" max="15" width="11.62890625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F1" t="s">
         <v>2</v>
       </c>
@@ -6600,7 +9673,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" t="s">
         <v>3</v>
       </c>
@@ -6622,12 +9695,12 @@
       <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="6"/>
+      <c r="Y2" s="5"/>
       <c r="Z2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F3">
         <f>H3*2*PI()*$P$1/G3</f>
         <v>20.943951023931955</v>
@@ -6646,12 +9719,12 @@
         <f>J3/K3</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y3" s="4"/>
+      <c r="Y3" s="3"/>
       <c r="Z3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F4">
         <f t="shared" ref="F4:F9" si="0">H4*2*PI()*$P$1/G4</f>
         <v>17.951958020513104</v>
@@ -6670,12 +9743,12 @@
         <f>J4/K4</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Y4" s="5"/>
+      <c r="Y4" s="4"/>
       <c r="Z4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F5">
         <f t="shared" si="0"/>
         <v>15.707963267948966</v>
@@ -6690,10 +9763,10 @@
       <c r="I5">
         <v>0.4</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="4">
         <v>3.8635000000000002</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K5" s="4">
         <v>5.8262999999999998</v>
       </c>
       <c r="L5">
@@ -6701,7 +9774,7 @@
         <v>0.66311381150987769</v>
       </c>
     </row>
-    <row r="6" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F6">
         <f t="shared" si="0"/>
         <v>13.962634015954636</v>
@@ -6716,16 +9789,16 @@
       <c r="I6">
         <v>0.45</v>
       </c>
-      <c r="J6" s="5">
+      <c r="J6" s="4">
         <v>2.8163999999999998</v>
       </c>
-      <c r="K6" s="5"/>
+      <c r="K6" s="4"/>
       <c r="L6" t="e">
         <f>J6/K6</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F7">
         <f t="shared" si="0"/>
         <v>12.566370614359172</v>
@@ -6740,10 +9813,10 @@
       <c r="I7">
         <v>0.5</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>2.2795000000000001</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <v>3.1558999999999999</v>
       </c>
       <c r="L7">
@@ -6751,7 +9824,7 @@
         <v>0.7222979181849869</v>
       </c>
     </row>
-    <row r="8" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F8">
         <f t="shared" si="0"/>
         <v>11.423973285781065</v>
@@ -6766,10 +9839,10 @@
       <c r="I8">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>1.7179</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>2.3298000000000001</v>
       </c>
       <c r="L8">
@@ -6777,7 +9850,7 @@
         <v>0.73735942999399084</v>
       </c>
     </row>
-    <row r="9" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F9">
         <f t="shared" si="0"/>
         <v>10.471975511965978</v>
@@ -6792,10 +9865,10 @@
       <c r="I9">
         <v>0.6</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>1.3338000000000001</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>1.7305999999999999</v>
       </c>
       <c r="L9">
@@ -6803,7 +9876,7 @@
         <v>0.77071535883508624</v>
       </c>
     </row>
-    <row r="11" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F11" t="s">
         <v>2</v>
       </c>
@@ -6811,7 +9884,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F12" t="s">
         <v>3</v>
       </c>
@@ -6834,7 +9907,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F13">
         <f>H13*2*PI()*$P$1/G13</f>
         <v>20.943951023931955</v>
@@ -6854,7 +9927,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F14">
         <f t="shared" ref="F14:F19" si="3">H14*2*PI()*$P$1/G14</f>
         <v>17.951958020513104</v>
@@ -6869,10 +9942,10 @@
       <c r="I14">
         <v>0.35</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <v>2.4007999999999998</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>3.5183</v>
       </c>
       <c r="L14">
@@ -6880,7 +9953,7 @@
         <v>0.68237501065855666</v>
       </c>
     </row>
-    <row r="15" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F15">
         <f t="shared" si="3"/>
         <v>15.707963267948966</v>
@@ -6895,10 +9968,10 @@
       <c r="I15">
         <v>0.4</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <v>1.5656000000000001</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="5">
         <v>2.1171000000000002</v>
       </c>
       <c r="L15">
@@ -6906,7 +9979,7 @@
         <v>0.73950214916631241</v>
       </c>
     </row>
-    <row r="16" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="6:26" x14ac:dyDescent="0.55000000000000004">
       <c r="F16">
         <f t="shared" si="3"/>
         <v>13.962634015954636</v>
@@ -6921,10 +9994,10 @@
       <c r="I16">
         <v>0.45</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="5">
         <v>1.0224</v>
       </c>
-      <c r="K16" s="6">
+      <c r="K16" s="5">
         <v>1.3049999999999999</v>
       </c>
       <c r="L16">
@@ -6932,7 +10005,7 @@
         <v>0.783448275862069</v>
       </c>
     </row>
-    <row r="17" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:12" x14ac:dyDescent="0.55000000000000004">
       <c r="F17">
         <f t="shared" si="3"/>
         <v>12.566370614359172</v>
@@ -6947,10 +10020,10 @@
       <c r="I17">
         <v>0.5</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="3">
         <v>0.65317999999999998</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="3">
         <v>0.80198999999999998</v>
       </c>
       <c r="L17">
@@ -6958,7 +10031,7 @@
         <v>0.8144490579683038</v>
       </c>
     </row>
-    <row r="18" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:12" x14ac:dyDescent="0.55000000000000004">
       <c r="F18">
         <f t="shared" si="3"/>
         <v>11.423973285781065</v>
@@ -6973,10 +10046,10 @@
       <c r="I18">
         <v>0.55000000000000004</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="5">
         <v>0.40433000000000002</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="5">
         <v>0.49051</v>
       </c>
       <c r="L18">
@@ -6984,7 +10057,7 @@
         <v>0.82430531487635328</v>
       </c>
     </row>
-    <row r="19" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:12" x14ac:dyDescent="0.55000000000000004">
       <c r="F19">
         <f t="shared" si="3"/>
         <v>10.471975511965978</v>
@@ -6999,10 +10072,10 @@
       <c r="I19">
         <v>0.6</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="5">
         <v>0.23685999999999999</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="5">
         <v>0.29032000000000002</v>
       </c>
       <c r="L19">

</xml_diff>

<commit_message>
Add README files for GA and Submodels directories to provide documentation on folder contents
</commit_message>
<xml_diff>
--- a/Validation/WindTunnelData.xlsx
+++ b/Validation/WindTunnelData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/B266C95A83FBF4BB/Documenten/TU Delft Aerospace Engineering/Msc2/AE5222 - Thesis/Software/Conceptual-Investigation-of-Alternative-Electric-Ducted-Fan-Architectures/Validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="826" documentId="8_{E7BF6703-466F-4498-AEEA-FFB8403C4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83F154ED-38A9-462A-B1C5-AE7E01864D49}"/>
+  <xr:revisionPtr revIDLastSave="1005" documentId="8_{E7BF6703-466F-4498-AEEA-FFB8403C4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06B417F6-E664-4C08-AC6B-3A69EF712914}"/>
   <bookViews>
     <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{6111FCF9-37F3-4199-9E4E-EEB7F0803D9A}"/>
   </bookViews>
@@ -74,44 +74,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>tc={0C73F34A-416F-4935-9E33-E2976851D391}</author>
-    <author>tc={7E06195D-819B-49FA-879C-2F5BADC7509B}</author>
-    <author>tc={490DC94F-35C6-41A8-8DB0-9F11B254BAD8}</author>
-  </authors>
-  <commentList>
-    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{0C73F34A-416F-4935-9E33-E2976851D391}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    No viscous solve completed</t>
-      </text>
-    </comment>
-    <comment ref="J7" authorId="1" shapeId="0" xr:uid="{7E06195D-819B-49FA-879C-2F5BADC7509B}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    No boundary layer on surface 3, unconverged boundary layer on element 2</t>
-      </text>
-    </comment>
-    <comment ref="J17" authorId="2" shapeId="0" xr:uid="{490DC94F-35C6-41A8-8DB0-9F11B254BAD8}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Solver does not converge. Peak residual 0.3e-3 (TE wake of duct)</t>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="30">
   <si>
     <t>CT</t>
   </si>
@@ -193,12 +157,22 @@
   <si>
     <t>Cpuncertainty</t>
   </si>
+  <si>
+    <t>No analysis performed</t>
+  </si>
+  <si>
+    <t>Note:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These results were gathered between 1-4-2025 and 2-4-2025. At this point, there was no functional crash handler or non-convergence handler.
+ For the more complete set of outputs, please refer to the last sheet of this file. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,14 +196,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +222,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -268,13 +242,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -825,51 +803,48 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$I$3:$I$9</c:f>
+              <c:f>'test results - with crash handl'!$I$3:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.3</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.6</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$K$3:$K$9</c:f>
+              <c:f>'test results - with crash handl'!$K$3:$K$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.6273</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0543999999999998</c:v>
+                </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8262999999999998</c:v>
+                  <c:v>2.3357000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7111000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1558999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.3298000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.6547000000000001</c:v>
+                  <c:v>1.1183000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -895,7 +870,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
+            <c:symbol val="circle"/>
             <c:size val="5"/>
             <c:spPr>
               <a:solidFill>
@@ -1220,7 +1195,6 @@
       <c:valAx>
         <c:axId val="923554783"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1587,57 +1561,48 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$I$13:$I$19</c:f>
+              <c:f>'test results - with crash handl'!$I$11:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.3</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.6</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$K$13:$K$19</c:f>
+              <c:f>'test results - with crash handl'!$K$11:$K$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1.2148000000000001</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5183</c:v>
+                  <c:v>0.76963999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1171000000000002</c:v>
+                  <c:v>0.48186000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3049999999999999</c:v>
+                  <c:v>0.28632000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.80198999999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.49051</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.29032000000000002</c:v>
+                  <c:v>0.13508999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1988,7 +1953,6 @@
       <c:valAx>
         <c:axId val="923554783"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6071,54 +6035,48 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$I$3:$I$9</c:f>
+              <c:f>'test results - with crash handl'!$I$3:$I$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.3</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.6</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$J$3:$J$9</c:f>
+              <c:f>'test results - with crash handl'!$J$3:$J$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.0316000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2250999999999999</c:v>
+                </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8635000000000002</c:v>
+                  <c:v>1.7265999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8163999999999998</c:v>
+                  <c:v>1.3222</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2795000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.7179</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.282</c:v>
+                  <c:v>0.93950999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6467,7 +6425,6 @@
       <c:valAx>
         <c:axId val="923554783"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6986,57 +6943,48 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$I$13:$I$19</c:f>
+              <c:f>'test results - with crash handl'!$I$11:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.3</c:v>
+                  <c:v>0.45</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.4</c:v>
+                  <c:v>0.55000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.45</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.55000000000000004</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.6</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$J$13:$J$19</c:f>
+              <c:f>'test results - with crash handl'!$J$11:$J$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.95596000000000003</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4007999999999998</c:v>
+                  <c:v>0.62936999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5656000000000001</c:v>
+                  <c:v>0.40209</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0224</c:v>
+                  <c:v>0.23738999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.65317999999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.40433000000000002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.23685999999999999</c:v>
+                  <c:v>0.10314</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7198,7 +7146,6 @@
       <c:valAx>
         <c:axId val="1167252687"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -13807,15 +13754,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>332740</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>8255</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>637540</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>161290</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -13845,15 +13792,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>313079</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>171027</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>630877</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>115141</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -13883,15 +13830,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>638794</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>300347</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>162560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -13921,15 +13868,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>627066</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>172241</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>28</xdr:col>
       <xdr:colOff>296883</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>134009</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -14379,26 +14326,12 @@
 </ThreadedComments>
 </file>
 
-<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
-<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="J6" dT="2025-04-01T21:08:09.20" personId="{1C3AF4B3-006D-4892-ABCA-8DF6491A77DD}" id="{0C73F34A-416F-4935-9E33-E2976851D391}">
-    <text>No viscous solve completed</text>
-  </threadedComment>
-  <threadedComment ref="J7" dT="2025-04-01T20:36:53.29" personId="{1C3AF4B3-006D-4892-ABCA-8DF6491A77DD}" id="{7E06195D-819B-49FA-879C-2F5BADC7509B}">
-    <text>No boundary layer on surface 3, unconverged boundary layer on element 2</text>
-  </threadedComment>
-  <threadedComment ref="J17" dT="2025-04-01T22:20:04.75" personId="{1C3AF4B3-006D-4892-ABCA-8DF6491A77DD}" id="{490DC94F-35C6-41A8-8DB0-9F11B254BAD8}">
-    <text>Solver does not converge. Peak residual 0.3e-3 (TE wake of duct)</text>
-  </threadedComment>
-</ThreadedComments>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B26E69B-6441-4D2A-91E2-CF3588D774EF}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5:L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15099,10 +15032,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D17483C-FDF0-45AC-9867-0493571C96AF}">
-  <dimension ref="F1:Z19"/>
+  <dimension ref="F1:AO19"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="72" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="AQ23" sqref="AQ23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15110,7 +15043,7 @@
     <col min="15" max="15" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F1" t="s">
         <v>2</v>
       </c>
@@ -15131,7 +15064,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F2" t="s">
         <v>3</v>
       </c>
@@ -15158,7 +15091,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F3">
         <f>H3*2*PI()*$P$1/G3</f>
         <v>20.943951023931955</v>
@@ -15182,7 +15115,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F4">
         <f t="shared" ref="F4:F9" si="0">H4*2*PI()*$P$1/G4</f>
         <v>17.951958020513104</v>
@@ -15206,7 +15139,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F5">
         <f t="shared" si="0"/>
         <v>15.707963267948966</v>
@@ -15232,7 +15165,7 @@
         <v>0.66311381150987769</v>
       </c>
     </row>
-    <row r="6" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F6">
         <f t="shared" si="0"/>
         <v>13.962634015954636</v>
@@ -15256,7 +15189,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F7">
         <f t="shared" si="0"/>
         <v>12.566370614359172</v>
@@ -15282,7 +15215,7 @@
         <v>0.7222979181849869</v>
       </c>
     </row>
-    <row r="8" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F8">
         <f t="shared" si="0"/>
         <v>11.423973285781065</v>
@@ -15308,7 +15241,7 @@
         <v>0.73735942999399084</v>
       </c>
     </row>
-    <row r="9" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F9">
         <f t="shared" si="0"/>
         <v>10.471975511965978</v>
@@ -15333,16 +15266,41 @@
         <f t="shared" si="2"/>
         <v>0.77071535883508624</v>
       </c>
+      <c r="AG9" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="11" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="6:41" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AG10" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="7"/>
+      <c r="AJ10" s="7"/>
+      <c r="AK10" s="7"/>
+      <c r="AL10" s="7"/>
+      <c r="AM10" s="7"/>
+      <c r="AN10" s="7"/>
+      <c r="AO10" s="7"/>
+    </row>
+    <row r="11" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F11" t="s">
         <v>2</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="7"/>
+      <c r="AI11" s="7"/>
+      <c r="AJ11" s="7"/>
+      <c r="AK11" s="7"/>
+      <c r="AL11" s="7"/>
+      <c r="AM11" s="7"/>
+      <c r="AN11" s="7"/>
+      <c r="AO11" s="7"/>
     </row>
-    <row r="12" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F12" t="s">
         <v>3</v>
       </c>
@@ -15365,7 +15323,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F13">
         <f>H13*2*PI()*$P$1/G13</f>
         <v>20.943951023931955</v>
@@ -15385,7 +15343,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F14">
         <f t="shared" ref="F14:F19" si="3">H14*2*PI()*$P$1/G14</f>
         <v>17.951958020513104</v>
@@ -15411,7 +15369,7 @@
         <v>0.68237501065855666</v>
       </c>
     </row>
-    <row r="15" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F15">
         <f t="shared" si="3"/>
         <v>15.707963267948966</v>
@@ -15437,7 +15395,7 @@
         <v>0.73950214916631241</v>
       </c>
     </row>
-    <row r="16" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F16">
         <f t="shared" si="3"/>
         <v>13.962634015954636</v>
@@ -15542,48 +15500,52 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="AG11:AO11"/>
+    <mergeCell ref="AG10:AO10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9A3C9B-DBC3-40D2-A144-241D094FABD6}">
-  <dimension ref="F1:Z19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9A3C9B-DBC3-40D2-A144-241D094FABD6}">
+  <dimension ref="F1:AA15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="72" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="72" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="15" max="15" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>5</v>
       </c>
-      <c r="P1">
+      <c r="Q1">
         <f>CONVERT(7,"ft","m")</f>
         <v>2.1335999999999999</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F2" t="s">
         <v>3</v>
       </c>
@@ -15605,398 +15567,317 @@
       <c r="L2" t="s">
         <v>8</v>
       </c>
-      <c r="Y2" s="5"/>
-      <c r="Z2" t="s">
+      <c r="Z2" s="5"/>
+      <c r="AA2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F3">
-        <f>H3*2*PI()*$P$1/G3</f>
-        <v>20.943951023931955</v>
+        <f>H3*2*PI()*$Q$1/G3</f>
+        <v>13.962634015954634</v>
       </c>
       <c r="G3">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H3">
-        <f>G3/(I3*$P$1)</f>
-        <v>43.744531933508313</v>
+        <f>G3/(I3*$Q$1)</f>
+        <v>36.453776611256927</v>
       </c>
       <c r="I3">
-        <v>0.3</v>
-      </c>
-      <c r="L3" t="e">
+        <v>0.45</v>
+      </c>
+      <c r="J3" s="5">
+        <v>3.0316000000000001</v>
+      </c>
+      <c r="K3" s="5">
+        <v>4.6273</v>
+      </c>
+      <c r="L3">
         <f>J3/K3</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y3" s="3"/>
-      <c r="Z3" t="s">
+        <v>0.65515527413394425</v>
+      </c>
+      <c r="Z3" s="3"/>
+      <c r="AA3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F4">
-        <f t="shared" ref="F4:F9" si="0">H4*2*PI()*$P$1/G4</f>
-        <v>17.951958020513104</v>
+        <f>H4*2*PI()*$Q$1/G4</f>
+        <v>12.566370614359172</v>
       </c>
       <c r="G4">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H9" si="1">G4/(I4*$P$1)</f>
-        <v>37.495313085864268</v>
+        <f>G4/(I4*$Q$1)</f>
+        <v>32.808398950131235</v>
       </c>
       <c r="I4">
-        <v>0.35</v>
-      </c>
-      <c r="L4" t="e">
-        <f>J4/K4</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="Y4" s="4"/>
-      <c r="Z4" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="J4" s="5">
+        <v>2.2250999999999999</v>
+      </c>
+      <c r="K4" s="5">
+        <v>3.0543999999999998</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L7" si="0">J4/K4</f>
+        <v>0.72849004714510213</v>
+      </c>
+      <c r="Z4" s="4"/>
+      <c r="AA4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="6:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F5">
+        <f>H5*2*PI()*$Q$1/G5</f>
+        <v>11.423973285781065</v>
+      </c>
+      <c r="G5">
+        <v>35</v>
+      </c>
+      <c r="H5">
+        <f>G5/(I5*$Q$1)</f>
+        <v>29.825817227392029</v>
+      </c>
+      <c r="I5">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J5" s="5">
+        <v>1.7265999999999999</v>
+      </c>
+      <c r="K5" s="5">
+        <v>2.3357000000000001</v>
+      </c>
+      <c r="L5">
         <f t="shared" si="0"/>
-        <v>15.707963267948966</v>
-      </c>
-      <c r="G5">
-        <v>28</v>
-      </c>
-      <c r="H5">
+        <v>0.73922164661557554</v>
+      </c>
+      <c r="Z5" s="6"/>
+      <c r="AA5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="F6">
+        <f>H6*2*PI()*$Q$1/G6</f>
+        <v>10.471975511965976</v>
+      </c>
+      <c r="G6">
+        <v>35</v>
+      </c>
+      <c r="H6">
+        <f>G6/(I6*$Q$1)</f>
+        <v>27.340332458442695</v>
+      </c>
+      <c r="I6">
+        <v>0.6</v>
+      </c>
+      <c r="J6" s="5">
+        <v>1.3222</v>
+      </c>
+      <c r="K6" s="5">
+        <v>1.7111000000000001</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0.77271930337209982</v>
+      </c>
+    </row>
+    <row r="7" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <f>H7*2*PI()*$Q$1/G7</f>
+        <v>9.6664389341224393</v>
+      </c>
+      <c r="G7">
+        <v>35</v>
+      </c>
+      <c r="H7">
+        <f>G7/(I7*$Q$1)</f>
+        <v>25.237229961639411</v>
+      </c>
+      <c r="I7">
+        <v>0.65</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0.93950999999999996</v>
+      </c>
+      <c r="K7" s="5">
+        <v>1.1183000000000001</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0.84012340159170162</v>
+      </c>
+    </row>
+    <row r="9" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="F11">
+        <f t="shared" ref="F11:F15" si="1">H11*2*PI()*$Q$1/G11</f>
+        <v>13.962634015954634</v>
+      </c>
+      <c r="G11">
+        <v>35</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ref="H11:H15" si="2">G11/(I11*$Q$1)</f>
+        <v>36.453776611256927</v>
+      </c>
+      <c r="I11">
+        <v>0.45</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0.95596000000000003</v>
+      </c>
+      <c r="K11" s="5">
+        <v>1.2148000000000001</v>
+      </c>
+      <c r="L11">
+        <f>J11/K11</f>
+        <v>0.78692788936450442</v>
+      </c>
+    </row>
+    <row r="12" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="F12">
         <f t="shared" si="1"/>
+        <v>12.566370614359172</v>
+      </c>
+      <c r="G12">
+        <v>35</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
         <v>32.808398950131235</v>
       </c>
-      <c r="I5">
-        <v>0.4</v>
-      </c>
-      <c r="J5" s="4">
-        <v>3.8635000000000002</v>
-      </c>
-      <c r="K5" s="4">
-        <v>5.8262999999999998</v>
-      </c>
-      <c r="L5">
-        <f>J5/K5</f>
-        <v>0.66311381150987769</v>
+      <c r="I12">
+        <v>0.5</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0.62936999999999999</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0.76963999999999999</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ref="L12:L15" si="3">J12/K12</f>
+        <v>0.81774595914973236</v>
       </c>
     </row>
-    <row r="6" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F6">
-        <f t="shared" si="0"/>
-        <v>13.962634015954636</v>
-      </c>
-      <c r="G6">
-        <v>28</v>
-      </c>
-      <c r="H6">
+    <row r="13" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="F13">
         <f t="shared" si="1"/>
-        <v>29.163021289005542</v>
-      </c>
-      <c r="I6">
-        <v>0.45</v>
-      </c>
-      <c r="J6" s="4">
-        <v>2.8163999999999998</v>
-      </c>
-      <c r="K6" s="4"/>
-      <c r="L6" t="e">
-        <f>J6/K6</f>
-        <v>#DIV/0!</v>
+        <v>11.423973285781065</v>
+      </c>
+      <c r="G13">
+        <v>35</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>29.825817227392029</v>
+      </c>
+      <c r="I13">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0.40209</v>
+      </c>
+      <c r="K13" s="5">
+        <v>0.48186000000000001</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="3"/>
+        <v>0.83445399078570537</v>
       </c>
     </row>
-    <row r="7" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F7">
-        <f t="shared" si="0"/>
-        <v>12.566370614359172</v>
-      </c>
-      <c r="G7">
-        <v>28</v>
-      </c>
-      <c r="H7">
+    <row r="14" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="F14">
         <f t="shared" si="1"/>
-        <v>26.246719160104988</v>
-      </c>
-      <c r="I7">
-        <v>0.5</v>
-      </c>
-      <c r="J7" s="3">
-        <v>2.2795000000000001</v>
-      </c>
-      <c r="K7" s="3">
-        <v>3.1558999999999999</v>
-      </c>
-      <c r="L7">
-        <f t="shared" ref="L7:L9" si="2">J7/K7</f>
-        <v>0.7222979181849869</v>
+        <v>10.471975511965976</v>
+      </c>
+      <c r="G14">
+        <v>35</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>27.340332458442695</v>
+      </c>
+      <c r="I14">
+        <v>0.6</v>
+      </c>
+      <c r="J14" s="5">
+        <v>0.23738999999999999</v>
+      </c>
+      <c r="K14" s="5">
+        <v>0.28632000000000002</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="3"/>
+        <v>0.82910729253981552</v>
       </c>
     </row>
-    <row r="8" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>11.423973285781065</v>
-      </c>
-      <c r="G8">
-        <v>28</v>
-      </c>
-      <c r="H8">
+    <row r="15" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="F15">
         <f t="shared" si="1"/>
-        <v>23.860653781913623</v>
-      </c>
-      <c r="I8">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="J8" s="5">
-        <v>1.7179</v>
-      </c>
-      <c r="K8" s="5">
-        <v>2.3298000000000001</v>
-      </c>
-      <c r="L8">
+        <v>9.6664389341224393</v>
+      </c>
+      <c r="G15">
+        <v>35</v>
+      </c>
+      <c r="H15">
         <f t="shared" si="2"/>
-        <v>0.73735942999399084</v>
-      </c>
-    </row>
-    <row r="9" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>10.471975511965978</v>
-      </c>
-      <c r="G9">
-        <v>28</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="1"/>
-        <v>21.872265966754156</v>
-      </c>
-      <c r="I9">
-        <v>0.6</v>
-      </c>
-      <c r="J9" s="5">
-        <v>1.282</v>
-      </c>
-      <c r="K9" s="5">
-        <v>1.6547000000000001</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="2"/>
-        <v>0.77476279688160998</v>
-      </c>
-    </row>
-    <row r="11" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F11" t="s">
-        <v>2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" t="s">
-        <v>9</v>
-      </c>
-      <c r="I12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>0</v>
-      </c>
-      <c r="K12" t="s">
-        <v>7</v>
-      </c>
-      <c r="L12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F13">
-        <f>H13*2*PI()*$P$1/G13</f>
-        <v>20.943951023931955</v>
-      </c>
-      <c r="G13">
-        <v>28</v>
-      </c>
-      <c r="H13">
-        <f>G13/(I13*$P$1)</f>
-        <v>43.744531933508313</v>
-      </c>
-      <c r="I13">
-        <v>0.3</v>
-      </c>
-      <c r="L13" t="e">
-        <f>J13/K13</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F14">
-        <f t="shared" ref="F14:F19" si="3">H14*2*PI()*$P$1/G14</f>
-        <v>17.951958020513104</v>
-      </c>
-      <c r="G14">
-        <v>28</v>
-      </c>
-      <c r="H14">
-        <f t="shared" ref="H14:H19" si="4">G14/(I14*$P$1)</f>
-        <v>37.495313085864268</v>
-      </c>
-      <c r="I14">
-        <v>0.35</v>
-      </c>
-      <c r="J14" s="5">
-        <v>2.4007999999999998</v>
-      </c>
-      <c r="K14" s="5">
-        <v>3.5183</v>
-      </c>
-      <c r="L14">
-        <f>J14/K14</f>
-        <v>0.68237501065855666</v>
-      </c>
-    </row>
-    <row r="15" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F15">
+        <v>25.237229961639411</v>
+      </c>
+      <c r="I15">
+        <v>0.65</v>
+      </c>
+      <c r="J15" s="5">
+        <v>0.10314</v>
+      </c>
+      <c r="K15" s="5">
+        <v>0.13508999999999999</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="3"/>
-        <v>15.707963267948966</v>
-      </c>
-      <c r="G15">
-        <v>28</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="4"/>
-        <v>32.808398950131235</v>
-      </c>
-      <c r="I15">
-        <v>0.4</v>
-      </c>
-      <c r="J15" s="5">
-        <v>1.5656000000000001</v>
-      </c>
-      <c r="K15" s="5">
-        <v>2.1171000000000002</v>
-      </c>
-      <c r="L15">
-        <f>J15/K15</f>
-        <v>0.73950214916631241</v>
-      </c>
-    </row>
-    <row r="16" spans="6:26" x14ac:dyDescent="0.35">
-      <c r="F16">
-        <f t="shared" si="3"/>
-        <v>13.962634015954636</v>
-      </c>
-      <c r="G16">
-        <v>28</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="4"/>
-        <v>29.163021289005542</v>
-      </c>
-      <c r="I16">
-        <v>0.45</v>
-      </c>
-      <c r="J16" s="5">
-        <v>1.0224</v>
-      </c>
-      <c r="K16" s="5">
-        <v>1.3049999999999999</v>
-      </c>
-      <c r="L16">
-        <f>J16/K16</f>
-        <v>0.783448275862069</v>
-      </c>
-    </row>
-    <row r="17" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F17">
-        <f t="shared" si="3"/>
-        <v>12.566370614359172</v>
-      </c>
-      <c r="G17">
-        <v>28</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="4"/>
-        <v>26.246719160104988</v>
-      </c>
-      <c r="I17">
-        <v>0.5</v>
-      </c>
-      <c r="J17" s="3">
-        <v>0.65317999999999998</v>
-      </c>
-      <c r="K17" s="3">
-        <v>0.80198999999999998</v>
-      </c>
-      <c r="L17">
-        <f t="shared" ref="L17:L19" si="5">J17/K17</f>
-        <v>0.8144490579683038</v>
-      </c>
-    </row>
-    <row r="18" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F18">
-        <f t="shared" si="3"/>
-        <v>11.423973285781065</v>
-      </c>
-      <c r="G18">
-        <v>28</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="4"/>
-        <v>23.860653781913623</v>
-      </c>
-      <c r="I18">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="J18" s="5">
-        <v>0.40433000000000002</v>
-      </c>
-      <c r="K18" s="5">
-        <v>0.49051</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="5"/>
-        <v>0.82430531487635328</v>
-      </c>
-    </row>
-    <row r="19" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F19">
-        <f t="shared" si="3"/>
-        <v>10.471975511965978</v>
-      </c>
-      <c r="G19">
-        <v>28</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="4"/>
-        <v>21.872265966754156</v>
-      </c>
-      <c r="I19">
-        <v>0.6</v>
-      </c>
-      <c r="J19" s="5">
-        <v>0.23685999999999999</v>
-      </c>
-      <c r="K19" s="5">
-        <v>0.29032000000000002</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="5"/>
-        <v>0.81585836318545046</v>
+        <v>0.76349100599600273</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adds optimization constraints and refactors objectives handling
Introduces a `Constraints` class for defining and computing optimization constraints, including equality and inequality types.
Refactors `Objectives` class to improve modularity and support dynamic objective computation.
Enhances `problem_definition` to integrate new constraints and objectives logic.
Removes legacy and unused files to clean up the codebase.
</commit_message>
<xml_diff>
--- a/Validation/WindTunnelData.xlsx
+++ b/Validation/WindTunnelData.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1005" documentId="8_{E7BF6703-466F-4498-AEEA-FFB8403C4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06B417F6-E664-4C08-AC6B-3A69EF712914}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="3" xr2:uid="{6111FCF9-37F3-4199-9E4E-EEB7F0803D9A}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="2" activeTab="3" xr2:uid="{6111FCF9-37F3-4199-9E4E-EEB7F0803D9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Wind Tunnel Beta=29deg data" sheetId="16" r:id="rId1"/>
@@ -15516,7 +15516,7 @@
   <dimension ref="F1:AA15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="72" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Update radial stations to start from 0.05 for improved interpolation and adjust validation parameters for better performance
</commit_message>
<xml_diff>
--- a/Validation/WindTunnelData.xlsx
+++ b/Validation/WindTunnelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/B266C95A83FBF4BB/Documenten/TU Delft Aerospace Engineering/Msc2/AE5222 - Thesis/Software/Conceptual-Investigation-of-Alternative-Electric-Ducted-Fan-Architectures/Validation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b266c95a83fbf4bb/Documenten/TU Delft Aerospace Engineering/Msc2/AE5222 - Thesis/Software/Conceptual-Investigation-of-Alternative-Electric-Ducted-Fan-Architectures/Validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1005" documentId="8_{E7BF6703-466F-4498-AEEA-FFB8403C4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06B417F6-E664-4C08-AC6B-3A69EF712914}"/>
+  <xr:revisionPtr revIDLastSave="1190" documentId="8_{E7BF6703-466F-4498-AEEA-FFB8403C4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03B17CBC-995A-4B9A-BC9E-4E12E3A507BD}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="2" activeTab="3" xr2:uid="{6111FCF9-37F3-4199-9E4E-EEB7F0803D9A}"/>
+    <workbookView xWindow="50600" yWindow="4470" windowWidth="28800" windowHeight="15200" firstSheet="2" activeTab="3" xr2:uid="{6111FCF9-37F3-4199-9E4E-EEB7F0803D9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Wind Tunnel Beta=29deg data" sheetId="16" r:id="rId1"/>
@@ -803,23 +803,32 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$I$3:$I$7</c:f>
+              <c:f>'test results - with crash handl'!$I$3:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>0.55000000000000004</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
@@ -827,24 +836,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$K$3:$K$7</c:f>
+              <c:f>'test results - with crash handl'!$K$3:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.6273</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0543999999999998</c:v>
+                  <c:v>9.6806000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3357000000000001</c:v>
+                  <c:v>5.7892000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7111000000000001</c:v>
+                  <c:v>3.9821</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1183000000000001</c:v>
+                  <c:v>3.2622</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7118</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2592000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1561,23 +1579,32 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$I$11:$I$15</c:f>
+              <c:f>'test results - with crash handl'!$I$14:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>0.55000000000000004</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
@@ -1585,24 +1612,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$K$11:$K$15</c:f>
+              <c:f>'test results - with crash handl'!$K$14:$K$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.2148000000000001</c:v>
+                  <c:v>6.1067999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76963999999999999</c:v>
+                  <c:v>3.5200999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.48186000000000001</c:v>
+                  <c:v>2.1392000000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.28632000000000002</c:v>
+                  <c:v>1.2854000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.13508999999999999</c:v>
+                  <c:v>0.81101999999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.50260000000000005</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.29807</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.14926</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6035,23 +6071,32 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$I$3:$I$7</c:f>
+              <c:f>'test results - with crash handl'!$I$3:$I$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>0.55000000000000004</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
@@ -6059,24 +6104,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$J$3:$J$7</c:f>
+              <c:f>'test results - with crash handl'!$J$3:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>3.0316000000000001</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2250999999999999</c:v>
+                  <c:v>5.4790999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7265999999999999</c:v>
+                  <c:v>3.8268</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3222</c:v>
+                  <c:v>2.8090000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.93950999999999996</c:v>
+                  <c:v>2.2841999999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7352000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.3211999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0087999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6943,23 +6997,32 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$I$11:$I$15</c:f>
+              <c:f>'test results - with crash handl'!$I$14:$I$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.45</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>0.5</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="5">
                   <c:v>0.55000000000000004</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>0.6</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
@@ -6967,24 +7030,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$J$11:$J$15</c:f>
+              <c:f>'test results - with crash handl'!$J$14:$J$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.95596000000000003</c:v>
+                  <c:v>3.7530999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.62936999999999999</c:v>
+                  <c:v>2.4028999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.40209</c:v>
+                  <c:v>1.5784</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.23738999999999999</c:v>
+                  <c:v>1.0024999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.10314</c:v>
+                  <c:v>0.65625</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.41277000000000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24399000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.10974</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13756,13 +13828,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>332740</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>8255</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>637540</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>161290</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -13794,13 +13866,13 @@
     <xdr:from>
       <xdr:col>13</xdr:col>
       <xdr:colOff>313079</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>171027</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>630877</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>115141</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -13832,13 +13904,13 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>638794</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>7620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>300347</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>162560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -13870,13 +13942,13 @@
     <xdr:from>
       <xdr:col>20</xdr:col>
       <xdr:colOff>627066</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>172241</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>28</xdr:col>
       <xdr:colOff>296883</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>134009</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -15513,10 +15585,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9A3C9B-DBC3-40D2-A144-241D094FABD6}">
-  <dimension ref="F1:AA15"/>
+  <dimension ref="F1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="72" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15572,60 +15644,60 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="6:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="6:27" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F3">
-        <f>H3*2*PI()*$Q$1/G3</f>
-        <v>13.962634015954634</v>
+        <f t="shared" ref="F3:F5" si="0">H3*2*PI()*$Q$1/G3</f>
+        <v>20.943951023931955</v>
       </c>
       <c r="G3">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H3">
         <f>G3/(I3*$Q$1)</f>
-        <v>36.453776611256927</v>
+        <v>46.869141357330335</v>
       </c>
       <c r="I3">
-        <v>0.45</v>
-      </c>
-      <c r="J3" s="5">
-        <v>3.0316000000000001</v>
-      </c>
-      <c r="K3" s="5">
-        <v>4.6273</v>
-      </c>
-      <c r="L3">
-        <f>J3/K3</f>
-        <v>0.65515527413394425</v>
+        <v>0.3</v>
+      </c>
+      <c r="J3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6">
+        <v>0</v>
+      </c>
+      <c r="L3" t="e">
+        <f t="shared" ref="L3:L4" si="1">J3/K3</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="Z3" s="3"/>
       <c r="AA3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="6:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="6:27" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F4">
-        <f>H4*2*PI()*$Q$1/G4</f>
-        <v>12.566370614359172</v>
+        <f t="shared" si="0"/>
+        <v>17.951958020513107</v>
       </c>
       <c r="G4">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H4">
         <f>G4/(I4*$Q$1)</f>
-        <v>32.808398950131235</v>
+        <v>40.173549734854575</v>
       </c>
       <c r="I4">
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="J4" s="5">
-        <v>2.2250999999999999</v>
+        <v>5.4790999999999999</v>
       </c>
       <c r="K4" s="5">
-        <v>3.0543999999999998</v>
+        <v>9.6806000000000001</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L7" si="0">J4/K4</f>
-        <v>0.72849004714510213</v>
+        <f t="shared" si="1"/>
+        <v>0.56598764539388058</v>
       </c>
       <c r="Z4" s="4"/>
       <c r="AA4" t="s">
@@ -15634,28 +15706,28 @@
     </row>
     <row r="5" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F5">
-        <f>H5*2*PI()*$Q$1/G5</f>
-        <v>11.423973285781065</v>
+        <f t="shared" si="0"/>
+        <v>15.707963267948966</v>
       </c>
       <c r="G5">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H5">
         <f>G5/(I5*$Q$1)</f>
-        <v>29.825817227392029</v>
+        <v>35.151856017997751</v>
       </c>
       <c r="I5">
-        <v>0.55000000000000004</v>
+        <v>0.4</v>
       </c>
       <c r="J5" s="5">
-        <v>1.7265999999999999</v>
+        <v>3.8268</v>
       </c>
       <c r="K5" s="5">
-        <v>2.3357000000000001</v>
+        <v>5.7892000000000001</v>
       </c>
       <c r="L5">
-        <f t="shared" si="0"/>
-        <v>0.73922164661557554</v>
+        <f>J5/K5</f>
+        <v>0.6610239756788503</v>
       </c>
       <c r="Z5" s="6"/>
       <c r="AA5" t="s">
@@ -15665,214 +15737,370 @@
     <row r="6" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F6">
         <f>H6*2*PI()*$Q$1/G6</f>
-        <v>10.471975511965976</v>
+        <v>13.962634015954638</v>
       </c>
       <c r="G6">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H6">
         <f>G6/(I6*$Q$1)</f>
-        <v>27.340332458442695</v>
+        <v>31.246094238220223</v>
       </c>
       <c r="I6">
-        <v>0.6</v>
+        <v>0.45</v>
       </c>
       <c r="J6" s="5">
-        <v>1.3222</v>
+        <v>2.8090000000000002</v>
       </c>
       <c r="K6" s="5">
-        <v>1.7111000000000001</v>
+        <v>3.9821</v>
       </c>
       <c r="L6">
-        <f t="shared" si="0"/>
-        <v>0.77271930337209982</v>
+        <f>J6/K6</f>
+        <v>0.70540669495994579</v>
       </c>
     </row>
     <row r="7" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F7">
-        <f>H7*2*PI()*$Q$1/G7</f>
-        <v>9.6664389341224393</v>
+        <f t="shared" ref="F7:F8" si="2">H7*2*PI()*$Q$1/G7</f>
+        <v>12.566370614359171</v>
       </c>
       <c r="G7">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H7">
         <f>G7/(I7*$Q$1)</f>
-        <v>25.237229961639411</v>
+        <v>28.121484814398201</v>
       </c>
       <c r="I7">
-        <v>0.65</v>
+        <v>0.5</v>
       </c>
       <c r="J7" s="5">
-        <v>0.93950999999999996</v>
+        <v>2.2841999999999998</v>
       </c>
       <c r="K7" s="5">
-        <v>1.1183000000000001</v>
+        <v>3.2622</v>
       </c>
       <c r="L7">
-        <f t="shared" si="0"/>
-        <v>0.84012340159170162</v>
+        <f t="shared" ref="L7:L10" si="3">J7/K7</f>
+        <v>0.70020231745447847</v>
+      </c>
+    </row>
+    <row r="8" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>11.423973285781065</v>
+      </c>
+      <c r="G8">
+        <v>30</v>
+      </c>
+      <c r="H8">
+        <f>G8/(I8*$Q$1)</f>
+        <v>25.564986194907451</v>
+      </c>
+      <c r="I8">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J8" s="5">
+        <v>1.7352000000000001</v>
+      </c>
+      <c r="K8" s="5">
+        <v>2.3512</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="3"/>
+        <v>0.73800612453215386</v>
       </c>
     </row>
     <row r="9" spans="6:27" x14ac:dyDescent="0.35">
-      <c r="F9" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" t="s">
-        <v>11</v>
+      <c r="F9">
+        <f>H9*2*PI()*$Q$1/G9</f>
+        <v>10.471975511965978</v>
+      </c>
+      <c r="G9">
+        <v>30</v>
+      </c>
+      <c r="H9">
+        <f>G9/(I9*$Q$1)</f>
+        <v>23.434570678665168</v>
+      </c>
+      <c r="I9">
+        <v>0.6</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1.3211999999999999</v>
+      </c>
+      <c r="K9" s="5">
+        <v>1.7118</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="3"/>
+        <v>0.77181913774973709</v>
       </c>
     </row>
     <row r="10" spans="6:27" x14ac:dyDescent="0.35">
-      <c r="F10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" t="s">
-        <v>9</v>
-      </c>
-      <c r="I10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" t="s">
-        <v>0</v>
-      </c>
-      <c r="K10" t="s">
-        <v>7</v>
-      </c>
-      <c r="L10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="6:27" x14ac:dyDescent="0.35">
-      <c r="F11">
-        <f t="shared" ref="F11:F15" si="1">H11*2*PI()*$Q$1/G11</f>
-        <v>13.962634015954634</v>
-      </c>
-      <c r="G11">
-        <v>35</v>
-      </c>
-      <c r="H11">
-        <f t="shared" ref="H11:H15" si="2">G11/(I11*$Q$1)</f>
-        <v>36.453776611256927</v>
-      </c>
-      <c r="I11">
-        <v>0.45</v>
-      </c>
-      <c r="J11" s="5">
-        <v>0.95596000000000003</v>
-      </c>
-      <c r="K11" s="5">
-        <v>1.2148000000000001</v>
-      </c>
-      <c r="L11">
-        <f>J11/K11</f>
-        <v>0.78692788936450442</v>
+      <c r="F10">
+        <f>H10*2*PI()*$Q$1/G10</f>
+        <v>9.666438934122441</v>
+      </c>
+      <c r="G10">
+        <v>30</v>
+      </c>
+      <c r="H10">
+        <f>G10/(I10*$Q$1)</f>
+        <v>21.631911395690921</v>
+      </c>
+      <c r="I10">
+        <v>0.65</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1.0087999999999999</v>
+      </c>
+      <c r="K10" s="5">
+        <v>1.2592000000000001</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="3"/>
+        <v>0.80114358322744583</v>
       </c>
     </row>
     <row r="12" spans="6:27" x14ac:dyDescent="0.35">
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>12.566370614359172</v>
-      </c>
-      <c r="G12">
-        <v>35</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="2"/>
-        <v>32.808398950131235</v>
-      </c>
-      <c r="I12">
-        <v>0.5</v>
-      </c>
-      <c r="J12" s="5">
-        <v>0.62936999999999999</v>
-      </c>
-      <c r="K12" s="5">
-        <v>0.76963999999999999</v>
-      </c>
-      <c r="L12">
-        <f t="shared" ref="L12:L15" si="3">J12/K12</f>
-        <v>0.81774595914973236</v>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="6:27" x14ac:dyDescent="0.35">
-      <c r="F13">
-        <f t="shared" si="1"/>
-        <v>11.423973285781065</v>
-      </c>
-      <c r="G13">
-        <v>35</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="2"/>
-        <v>29.825817227392029</v>
-      </c>
-      <c r="I13">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="J13" s="5">
-        <v>0.40209</v>
-      </c>
-      <c r="K13" s="5">
-        <v>0.48186000000000001</v>
-      </c>
-      <c r="L13">
-        <f t="shared" si="3"/>
-        <v>0.83445399078570537</v>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>4</v>
+      </c>
+      <c r="H13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I13" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>0</v>
+      </c>
+      <c r="K13" t="s">
+        <v>7</v>
+      </c>
+      <c r="L13" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F14">
-        <f t="shared" si="1"/>
-        <v>10.471975511965976</v>
+        <f t="shared" ref="F14" si="4">H14*2*PI()*$Q$1/G14</f>
+        <v>20.943951023931955</v>
       </c>
       <c r="G14">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H14">
-        <f t="shared" si="2"/>
-        <v>27.340332458442695</v>
+        <f t="shared" ref="H14" si="5">G14/(I14*$Q$1)</f>
+        <v>46.869141357330335</v>
       </c>
       <c r="I14">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="J14" s="5">
-        <v>0.23738999999999999</v>
+        <v>3.7530999999999999</v>
       </c>
       <c r="K14" s="5">
-        <v>0.28632000000000002</v>
+        <v>6.1067999999999998</v>
       </c>
       <c r="L14">
-        <f t="shared" si="3"/>
-        <v>0.82910729253981552</v>
+        <f>J14/K14</f>
+        <v>0.61457719263771537</v>
       </c>
     </row>
     <row r="15" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F15">
-        <f t="shared" si="1"/>
-        <v>9.6664389341224393</v>
+        <f t="shared" ref="F15:F21" si="6">H15*2*PI()*$Q$1/G15</f>
+        <v>17.951958020513107</v>
       </c>
       <c r="G15">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="H15">
-        <f t="shared" si="2"/>
-        <v>25.237229961639411</v>
+        <f t="shared" ref="H15:H21" si="7">G15/(I15*$Q$1)</f>
+        <v>40.173549734854575</v>
       </c>
       <c r="I15">
+        <v>0.35</v>
+      </c>
+      <c r="J15" s="5">
+        <v>2.4028999999999998</v>
+      </c>
+      <c r="K15" s="5">
+        <v>3.5200999999999998</v>
+      </c>
+      <c r="L15">
+        <f>J15/K15</f>
+        <v>0.68262265276554646</v>
+      </c>
+    </row>
+    <row r="16" spans="6:27" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <f t="shared" si="6"/>
+        <v>15.707963267948966</v>
+      </c>
+      <c r="G16">
+        <v>30</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="7"/>
+        <v>35.151856017997751</v>
+      </c>
+      <c r="I16">
+        <v>0.4</v>
+      </c>
+      <c r="J16" s="5">
+        <v>1.5784</v>
+      </c>
+      <c r="K16" s="5">
+        <v>2.1392000000000002</v>
+      </c>
+      <c r="L16">
+        <f>J16/K16</f>
+        <v>0.73784592370979796</v>
+      </c>
+    </row>
+    <row r="17" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F17">
+        <f t="shared" si="6"/>
+        <v>13.962634015954638</v>
+      </c>
+      <c r="G17">
+        <v>30</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="7"/>
+        <v>31.246094238220223</v>
+      </c>
+      <c r="I17">
+        <v>0.45</v>
+      </c>
+      <c r="J17" s="5">
+        <v>1.0024999999999999</v>
+      </c>
+      <c r="K17" s="5">
+        <v>1.2854000000000001</v>
+      </c>
+      <c r="L17">
+        <f>J17/K17</f>
+        <v>0.77991286758985523</v>
+      </c>
+    </row>
+    <row r="18" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F18">
+        <f t="shared" si="6"/>
+        <v>12.566370614359171</v>
+      </c>
+      <c r="G18">
+        <v>30</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="7"/>
+        <v>28.121484814398201</v>
+      </c>
+      <c r="I18">
+        <v>0.5</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0.65625</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0.81101999999999996</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18:L21" si="8">J18/K18</f>
+        <v>0.80916623511134134</v>
+      </c>
+    </row>
+    <row r="19" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F19">
+        <f t="shared" si="6"/>
+        <v>11.423973285781065</v>
+      </c>
+      <c r="G19">
+        <v>30</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="7"/>
+        <v>25.564986194907451</v>
+      </c>
+      <c r="I19">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0.41277000000000003</v>
+      </c>
+      <c r="K19" s="5">
+        <v>0.50260000000000005</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="8"/>
+        <v>0.82126939912455232</v>
+      </c>
+    </row>
+    <row r="20" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F20">
+        <f t="shared" si="6"/>
+        <v>10.471975511965978</v>
+      </c>
+      <c r="G20">
+        <v>30</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="7"/>
+        <v>23.434570678665168</v>
+      </c>
+      <c r="I20">
+        <v>0.6</v>
+      </c>
+      <c r="J20" s="5">
+        <v>0.24399000000000001</v>
+      </c>
+      <c r="K20" s="5">
+        <v>0.29807</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="8"/>
+        <v>0.81856610863220047</v>
+      </c>
+    </row>
+    <row r="21" spans="6:12" x14ac:dyDescent="0.35">
+      <c r="F21">
+        <f t="shared" si="6"/>
+        <v>9.666438934122441</v>
+      </c>
+      <c r="G21">
+        <v>30</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="7"/>
+        <v>21.631911395690921</v>
+      </c>
+      <c r="I21">
         <v>0.65</v>
       </c>
-      <c r="J15" s="5">
-        <v>0.10314</v>
-      </c>
-      <c r="K15" s="5">
-        <v>0.13508999999999999</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="3"/>
-        <v>0.76349100599600273</v>
+      <c r="J21" s="5">
+        <v>0.10974</v>
+      </c>
+      <c r="K21" s="5">
+        <v>0.14926</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="8"/>
+        <v>0.73522712046094063</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update advance ratio and freestream velocity in X22A_validator.py for improved validation accuracy
</commit_message>
<xml_diff>
--- a/Validation/WindTunnelData.xlsx
+++ b/Validation/WindTunnelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b266c95a83fbf4bb/Documenten/TU Delft Aerospace Engineering/Msc2/AE5222 - Thesis/Software/Conceptual-Investigation-of-Alternative-Electric-Ducted-Fan-Architectures/Validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1190" documentId="8_{E7BF6703-466F-4498-AEEA-FFB8403C4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03B17CBC-995A-4B9A-BC9E-4E12E3A507BD}"/>
+  <xr:revisionPtr revIDLastSave="1585" documentId="8_{E7BF6703-466F-4498-AEEA-FFB8403C4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F76418B-819D-4D34-B006-8FC6AE60D8D6}"/>
   <bookViews>
-    <workbookView xWindow="50600" yWindow="4470" windowWidth="28800" windowHeight="15200" firstSheet="2" activeTab="3" xr2:uid="{6111FCF9-37F3-4199-9E4E-EEB7F0803D9A}"/>
+    <workbookView xWindow="14325" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="3" xr2:uid="{6111FCF9-37F3-4199-9E4E-EEB7F0803D9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Wind Tunnel Beta=29deg data" sheetId="16" r:id="rId1"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="34">
   <si>
     <t>CT</t>
   </si>
@@ -167,12 +167,24 @@
     <t xml:space="preserve">These results were gathered between 1-4-2025 and 2-4-2025. At this point, there was no functional crash handler or non-convergence handler.
  For the more complete set of outputs, please refer to the last sheet of this file. </t>
   </si>
+  <si>
+    <t>TC</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>CT_error</t>
+  </si>
+  <si>
+    <t>CP_error</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +204,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -242,7 +261,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -253,6 +272,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -803,10 +823,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$I$3:$I$10</c:f>
+              <c:f>'test results - with crash handl'!$I$3:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.3</c:v>
                 </c:pt>
@@ -827,42 +847,30 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$K$3:$K$10</c:f>
+              <c:f>'test results - with crash handl'!$K$3:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.6806000000000001</c:v>
-                </c:pt>
+                <c:ptCount val="7"/>
                 <c:pt idx="2">
-                  <c:v>5.7892000000000001</c:v>
+                  <c:v>6.3601000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.9821</c:v>
+                  <c:v>4.5932000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.2622</c:v>
+                  <c:v>3.19</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.3512</c:v>
+                  <c:v>2.2608999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.7118</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.2592000000000001</c:v>
+                  <c:v>1.6632</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1270,7 +1278,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Coefficient CP </a:t>
+                  <a:t> Coefficient PC </a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB"/>
@@ -1579,10 +1587,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$I$14:$I$21</c:f>
+              <c:f>'test results - with crash handl'!$I$13:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.3</c:v>
                 </c:pt>
@@ -1603,42 +1611,36 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$K$14:$K$21</c:f>
+              <c:f>'test results - with crash handl'!$K$13:$K$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6.1067999999999998</c:v>
+                  <c:v>6.1909999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5200999999999998</c:v>
+                  <c:v>3.6280000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1392000000000002</c:v>
+                  <c:v>2.2471999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2854000000000001</c:v>
+                  <c:v>1.3714</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.81101999999999996</c:v>
+                  <c:v>0.86065999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.50260000000000005</c:v>
+                  <c:v>0.54393999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.29807</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.14926</c:v>
+                  <c:v>0.31189</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2046,11 +2048,1415 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Coefficient CP </a:t>
+                  <a:t> Coefficient PC </a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB"/>
                   <a:t>[-]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="923558143"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Comparison for </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="el-GR" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>β</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>=29</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Grotesque" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>˚</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MTFLOW</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'test results - with crash handl'!$I$3:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'test results - with crash handl'!$M$3:$M$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32695200000000008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30411450000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27928750000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.253237875</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23149799999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BCB6-47E2-8350-4E92094BF5B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Wind Tunnel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1.0000000000000002E-2"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1.0000000000000002E-2"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wind Tunnel Beta=29deg data'!$G$6:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wind Tunnel Beta=29deg data'!$B$6:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.37369999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.246</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BCB6-47E2-8350-4E92094BF5B5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="923558143"/>
+        <c:axId val="923554783"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="923558143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Advance Ratio J [-]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="923554783"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="923554783"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Thrust Coefficeint CT [-]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="923558143"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="LID4096"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="LID4096"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Comparison for </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="el-GR" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>β</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>=19</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="Grotesque" panose="020B0504020202020204" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>˚</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-GB"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>MTFLOW</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'test results - with crash handl'!$I$3:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'test results - with crash handl'!$M$13:$M$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.17118899999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14933974999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13156000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.108043875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.6684999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8118462500000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.5963000000000004E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D65B-4CE6-9223-554C6449EF73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Wind Tunnel</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1.0000000000000002E-2"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1.0000000000000002E-2"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Wind Tunnel Beta=19deg data'!$G$6:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Wind Tunnel Beta=19deg data'!$B$6:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.16950000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14949999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13070000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.1119</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.9349999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.1819999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D65B-4CE6-9223-554C6449EF73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="923558143"/>
+        <c:axId val="923554783"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="923558143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Advance Ratio J [-]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="LID4096"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="LID4096"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="923554783"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="923554783"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Thrust Coefficeint CT [-]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6071,10 +7477,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$I$3:$I$10</c:f>
+              <c:f>'test results - with crash handl'!$I$3:$I$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.3</c:v>
                 </c:pt>
@@ -6095,42 +7501,30 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$J$3:$J$10</c:f>
+              <c:f>'test results - with crash handl'!$J$4:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
+                <c:ptCount val="6"/>
                 <c:pt idx="1">
-                  <c:v>5.4790999999999999</c:v>
+                  <c:v>4.0869</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.8268</c:v>
+                  <c:v>3.0036</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8090000000000002</c:v>
+                  <c:v>2.2343000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2841999999999998</c:v>
+                  <c:v>1.6742999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7352000000000001</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.3211999999999999</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.0087999999999999</c:v>
+                  <c:v>1.2861</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6532,7 +7926,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Thrust Coefficeint CT [-]</a:t>
+                  <a:t>Thrust Coefficeint TC [-]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6997,10 +8391,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$I$14:$I$21</c:f>
+              <c:f>'test results - with crash handl'!$I$13:$I$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0.3</c:v>
                 </c:pt>
@@ -7021,42 +8415,36 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.6</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$J$14:$J$21</c:f>
+              <c:f>'test results - with crash handl'!$J$13:$J$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.7530999999999999</c:v>
+                  <c:v>3.8041999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4028999999999998</c:v>
+                  <c:v>2.4382000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5784</c:v>
+                  <c:v>1.6445000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0024999999999999</c:v>
+                  <c:v>1.0670999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.65625</c:v>
+                  <c:v>0.69347999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.41277000000000003</c:v>
+                  <c:v>0.45036999999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.24399000000000001</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.10974</c:v>
+                  <c:v>0.25535000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7275,7 +8663,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Coefficient CT [-]</a:t>
+                  <a:t> Coefficient TC [-]</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -7508,6 +8896,86 @@
 </file>
 
 <file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors13.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -9415,6 +10883,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style13.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -13826,16 +16326,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>332740</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>537045</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>8255</xdr:rowOff>
+      <xdr:rowOff>24821</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>637540</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>161290</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>413358</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>177856</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13864,16 +16364,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>313079</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>171027</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>517384</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>5376</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>630877</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>115141</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>413045</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>131707</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13902,16 +16402,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>638794</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>408261</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>7620</xdr:rowOff>
+      <xdr:rowOff>24186</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>300347</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>162560</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>101565</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>179126</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13940,16 +16440,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>627066</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>172241</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>409234</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>6590</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>296883</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>134009</xdr:rowOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>98101</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>150575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -13971,6 +16471,82 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>527709</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>155452</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>413637</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>105286</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B89EBB6-772E-45EC-ABEA-70B69A781111}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>579782</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>138043</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>465711</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>87877</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C8E8DD53-5F51-4C73-970E-B79C8DFB1CBA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -14403,27 +16979,27 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -14431,7 +17007,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -14463,7 +17039,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>0.3</v>
       </c>
@@ -14502,7 +17078,7 @@
         <v>0.74074074074074081</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>0.35</v>
       </c>
@@ -14541,7 +17117,7 @@
         <v>0.46647230320699723</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>0.4</v>
       </c>
@@ -14580,7 +17156,7 @@
         <v>0.31249999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>0.45</v>
       </c>
@@ -14619,7 +17195,7 @@
         <v>0.21947873799725648</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>0.5</v>
       </c>
@@ -14658,7 +17234,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>0.55000000000000004</v>
       </c>
@@ -14697,7 +17273,7 @@
         <v>0.12021036814425241</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>0.6</v>
       </c>
@@ -14755,27 +17331,27 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -14783,7 +17359,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -14815,7 +17391,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <v>0.3</v>
       </c>
@@ -14854,7 +17430,7 @@
         <v>0.74074074074074081</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <v>0.35</v>
       </c>
@@ -14893,7 +17469,7 @@
         <v>0.46647230320699723</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <v>0.4</v>
       </c>
@@ -14932,7 +17508,7 @@
         <v>0.31249999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <v>0.45</v>
       </c>
@@ -14971,7 +17547,7 @@
         <v>0.21947873799725648</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <v>0.5</v>
       </c>
@@ -15010,7 +17586,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <v>0.55000000000000004</v>
       </c>
@@ -15049,7 +17625,7 @@
         <v>0.12021036814425241</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <v>0.6</v>
       </c>
@@ -15107,15 +17683,15 @@
   <dimension ref="F1:AO19"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="72" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="AQ23" sqref="AQ23"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="15" max="15" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="1" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F1" t="s">
         <v>2</v>
       </c>
@@ -15136,7 +17712,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="2" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" t="s">
         <v>3</v>
       </c>
@@ -15163,7 +17739,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="3" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F3">
         <f>H3*2*PI()*$P$1/G3</f>
         <v>20.943951023931955</v>
@@ -15187,7 +17763,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="4" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F4">
         <f t="shared" ref="F4:F9" si="0">H4*2*PI()*$P$1/G4</f>
         <v>17.951958020513104</v>
@@ -15211,7 +17787,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="5" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F5">
         <f t="shared" si="0"/>
         <v>15.707963267948966</v>
@@ -15237,7 +17813,7 @@
         <v>0.66311381150987769</v>
       </c>
     </row>
-    <row r="6" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="6" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F6">
         <f t="shared" si="0"/>
         <v>13.962634015954636</v>
@@ -15261,7 +17837,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="7" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F7">
         <f t="shared" si="0"/>
         <v>12.566370614359172</v>
@@ -15287,7 +17863,7 @@
         <v>0.7222979181849869</v>
       </c>
     </row>
-    <row r="8" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="8" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F8">
         <f t="shared" si="0"/>
         <v>11.423973285781065</v>
@@ -15313,7 +17889,7 @@
         <v>0.73735942999399084</v>
       </c>
     </row>
-    <row r="9" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="9" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F9">
         <f t="shared" si="0"/>
         <v>10.471975511965978</v>
@@ -15342,7 +17918,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="6:41" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="6:41" ht="65.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="AG10" s="7" t="s">
         <v>29</v>
       </c>
@@ -15355,7 +17931,7 @@
       <c r="AN10" s="7"/>
       <c r="AO10" s="7"/>
     </row>
-    <row r="11" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="11" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F11" t="s">
         <v>2</v>
       </c>
@@ -15372,7 +17948,7 @@
       <c r="AN11" s="7"/>
       <c r="AO11" s="7"/>
     </row>
-    <row r="12" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="12" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F12" t="s">
         <v>3</v>
       </c>
@@ -15395,7 +17971,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="13" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F13">
         <f>H13*2*PI()*$P$1/G13</f>
         <v>20.943951023931955</v>
@@ -15415,7 +17991,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="14" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F14">
         <f t="shared" ref="F14:F19" si="3">H14*2*PI()*$P$1/G14</f>
         <v>17.951958020513104</v>
@@ -15441,7 +18017,7 @@
         <v>0.68237501065855666</v>
       </c>
     </row>
-    <row r="15" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="15" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F15">
         <f t="shared" si="3"/>
         <v>15.707963267948966</v>
@@ -15467,7 +18043,7 @@
         <v>0.73950214916631241</v>
       </c>
     </row>
-    <row r="16" spans="6:41" x14ac:dyDescent="0.35">
+    <row r="16" spans="6:41" x14ac:dyDescent="0.55000000000000004">
       <c r="F16">
         <f t="shared" si="3"/>
         <v>13.962634015954636</v>
@@ -15493,7 +18069,7 @@
         <v>0.783448275862069</v>
       </c>
     </row>
-    <row r="17" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:12" x14ac:dyDescent="0.55000000000000004">
       <c r="F17">
         <f t="shared" si="3"/>
         <v>12.566370614359172</v>
@@ -15519,7 +18095,7 @@
         <v>0.8144490579683038</v>
       </c>
     </row>
-    <row r="18" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:12" x14ac:dyDescent="0.55000000000000004">
       <c r="F18">
         <f t="shared" si="3"/>
         <v>11.423973285781065</v>
@@ -15545,7 +18121,7 @@
         <v>0.82430531487635328</v>
       </c>
     </row>
-    <row r="19" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:12" x14ac:dyDescent="0.55000000000000004">
       <c r="F19">
         <f t="shared" si="3"/>
         <v>10.471975511965978</v>
@@ -15585,18 +18161,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9A3C9B-DBC3-40D2-A144-241D094FABD6}">
-  <dimension ref="F1:AA21"/>
+  <dimension ref="F1:AA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="72" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="158" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J10" sqref="I10:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="16" max="16" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="6:27" x14ac:dyDescent="0.55000000000000004">
       <c r="F1" t="s">
         <v>2</v>
       </c>
@@ -15617,7 +18193,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="6:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="6:27" x14ac:dyDescent="0.55000000000000004">
       <c r="F2" t="s">
         <v>3</v>
       </c>
@@ -15631,481 +18207,669 @@
         <v>1</v>
       </c>
       <c r="J2" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s">
         <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>33</v>
       </c>
       <c r="Z2" s="5"/>
       <c r="AA2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="6:27" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="6:27" ht="14.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F3">
         <f t="shared" ref="F3:F5" si="0">H3*2*PI()*$Q$1/G3</f>
         <v>20.943951023931955</v>
       </c>
       <c r="G3">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H3">
-        <f>G3/(I3*$Q$1)</f>
-        <v>46.869141357330335</v>
+        <f t="shared" ref="H3:H9" si="1">G3/(I3*$Q$1)</f>
+        <v>40.61992250968629</v>
       </c>
       <c r="I3">
         <v>0.3</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" t="e">
+        <f>#REF!/K3</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M3" t="e">
+        <f>#REF!*POWER(I3,2)/2</f>
+        <v>#REF!</v>
+      </c>
+      <c r="N3">
+        <f>K3*POWER(I3,3)/2</f>
         <v>0</v>
       </c>
-      <c r="K3" s="6">
-        <v>0</v>
-      </c>
-      <c r="L3" t="e">
-        <f t="shared" ref="L3:L4" si="1">J3/K3</f>
-        <v>#DIV/0!</v>
+      <c r="O3" t="e">
+        <f>ABS(M3-'Wind Tunnel Beta=29deg data'!B6)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="P3">
+        <f>ABS(N3-'Wind Tunnel Beta=29deg data'!C6)</f>
+        <v>0.2412</v>
       </c>
       <c r="Z3" s="3"/>
       <c r="AA3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="6:27" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="6:27" ht="14.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>17.951958020513107</v>
+        <v>17.951958020513104</v>
       </c>
       <c r="G4">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H4">
-        <f>G4/(I4*$Q$1)</f>
-        <v>40.173549734854575</v>
+        <f t="shared" si="1"/>
+        <v>34.817076436873961</v>
       </c>
       <c r="I4">
         <v>0.35</v>
       </c>
-      <c r="J4" s="5">
-        <v>5.4790999999999999</v>
-      </c>
-      <c r="K4" s="5">
-        <v>9.6806000000000001</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="1"/>
-        <v>0.56598764539388058</v>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" t="e">
+        <f>J4/K4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M4">
+        <f>J4*POWER(I4,2)/2</f>
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N9" si="2">K4*POWER(I4,3)/2</f>
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <f>ABS(M4-'Wind Tunnel Beta=29deg data'!B7)</f>
+        <v>0.35</v>
+      </c>
+      <c r="P4">
+        <f>ABS(N4-'Wind Tunnel Beta=29deg data'!C7)</f>
+        <v>0.23649999999999999</v>
       </c>
       <c r="Z4" s="4"/>
       <c r="AA4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="6:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="6:27" x14ac:dyDescent="0.55000000000000004">
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>15.707963267948966</v>
+        <v>15.707963267948967</v>
       </c>
       <c r="G5">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H5">
-        <f>G5/(I5*$Q$1)</f>
-        <v>35.151856017997751</v>
+        <f t="shared" si="1"/>
+        <v>30.464941882264718</v>
       </c>
       <c r="I5">
         <v>0.4</v>
       </c>
       <c r="J5" s="5">
-        <v>3.8268</v>
+        <v>4.0869</v>
       </c>
       <c r="K5" s="5">
-        <v>5.7892000000000001</v>
+        <v>6.3601000000000001</v>
       </c>
       <c r="L5">
         <f>J5/K5</f>
-        <v>0.6610239756788503</v>
+        <v>0.64258423609691673</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M4:M9" si="3">J5*POWER(I5,2)/2</f>
+        <v>0.32695200000000008</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>0.20352320000000004</v>
+      </c>
+      <c r="O5">
+        <f>ABS(M5-'Wind Tunnel Beta=29deg data'!B8)</f>
+        <v>6.9520000000000692E-3</v>
+      </c>
+      <c r="P5">
+        <f>ABS(N5-'Wind Tunnel Beta=29deg data'!C8)</f>
+        <v>2.5576799999999955E-2</v>
       </c>
       <c r="Z5" s="6"/>
       <c r="AA5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="6:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="6:27" x14ac:dyDescent="0.55000000000000004">
       <c r="F6">
         <f>H6*2*PI()*$Q$1/G6</f>
-        <v>13.962634015954638</v>
+        <v>13.962634015954636</v>
       </c>
       <c r="G6">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H6">
-        <f>G6/(I6*$Q$1)</f>
-        <v>31.246094238220223</v>
+        <f t="shared" si="1"/>
+        <v>27.07994833979086</v>
       </c>
       <c r="I6">
         <v>0.45</v>
       </c>
       <c r="J6" s="5">
-        <v>2.8090000000000002</v>
+        <v>3.0036</v>
       </c>
       <c r="K6" s="5">
-        <v>3.9821</v>
+        <v>4.5932000000000004</v>
       </c>
       <c r="L6">
         <f>J6/K6</f>
-        <v>0.70540669495994579</v>
+        <v>0.65392319080379691</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>0.30411450000000001</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>0.20927767500000005</v>
+      </c>
+      <c r="O6">
+        <f>ABS(M6-'Wind Tunnel Beta=29deg data'!B9)</f>
+        <v>8.1145000000000245E-3</v>
+      </c>
+      <c r="P6">
+        <f>ABS(N6-'Wind Tunnel Beta=29deg data'!C9)</f>
+        <v>1.2422324999999956E-2</v>
       </c>
     </row>
-    <row r="7" spans="6:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="6:27" x14ac:dyDescent="0.55000000000000004">
       <c r="F7">
-        <f t="shared" ref="F7:F8" si="2">H7*2*PI()*$Q$1/G7</f>
-        <v>12.566370614359171</v>
+        <f t="shared" ref="F7:F8" si="4">H7*2*PI()*$Q$1/G7</f>
+        <v>12.566370614359174</v>
       </c>
       <c r="G7">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H7">
-        <f>G7/(I7*$Q$1)</f>
-        <v>28.121484814398201</v>
+        <f t="shared" si="1"/>
+        <v>24.371953505811774</v>
       </c>
       <c r="I7">
         <v>0.5</v>
       </c>
       <c r="J7" s="5">
-        <v>2.2841999999999998</v>
+        <v>2.2343000000000002</v>
       </c>
       <c r="K7" s="5">
-        <v>3.2622</v>
+        <v>3.19</v>
       </c>
       <c r="L7">
-        <f t="shared" ref="L7:L10" si="3">J7/K7</f>
-        <v>0.70020231745447847</v>
+        <f t="shared" ref="L7:L9" si="5">J7/K7</f>
+        <v>0.70040752351097191</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>0.27928750000000002</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>0.199375</v>
+      </c>
+      <c r="O7">
+        <f>ABS(M7-'Wind Tunnel Beta=29deg data'!B10)</f>
+        <v>9.2875000000000041E-3</v>
+      </c>
+      <c r="P7">
+        <f>ABS(N7-'Wind Tunnel Beta=29deg data'!C10)</f>
+        <v>1.5025000000000011E-2</v>
       </c>
     </row>
-    <row r="8" spans="6:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="6:27" x14ac:dyDescent="0.55000000000000004">
       <c r="F8">
-        <f t="shared" si="2"/>
-        <v>11.423973285781065</v>
+        <f t="shared" si="4"/>
+        <v>11.423973285781063</v>
       </c>
       <c r="G8">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H8">
-        <f>G8/(I8*$Q$1)</f>
-        <v>25.564986194907451</v>
+        <f t="shared" si="1"/>
+        <v>22.156321368919791</v>
       </c>
       <c r="I8">
         <v>0.55000000000000004</v>
       </c>
       <c r="J8" s="5">
-        <v>1.7352000000000001</v>
+        <v>1.6742999999999999</v>
       </c>
       <c r="K8" s="5">
-        <v>2.3512</v>
+        <v>2.2608999999999999</v>
       </c>
       <c r="L8">
+        <f t="shared" si="5"/>
+        <v>0.74054580034499529</v>
+      </c>
+      <c r="M8">
         <f t="shared" si="3"/>
-        <v>0.73800612453215386</v>
+        <v>0.253237875</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="2"/>
+        <v>0.18807861875000004</v>
+      </c>
+      <c r="O8">
+        <f>ABS(M8-'Wind Tunnel Beta=29deg data'!B11)</f>
+        <v>7.2378750000000047E-3</v>
+      </c>
+      <c r="P8">
+        <f>ABS(N8-'Wind Tunnel Beta=29deg data'!C11)</f>
+        <v>1.592138124999995E-2</v>
       </c>
     </row>
-    <row r="9" spans="6:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="6:27" x14ac:dyDescent="0.55000000000000004">
       <c r="F9">
         <f>H9*2*PI()*$Q$1/G9</f>
         <v>10.471975511965978</v>
       </c>
       <c r="G9">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H9">
-        <f>G9/(I9*$Q$1)</f>
-        <v>23.434570678665168</v>
+        <f t="shared" si="1"/>
+        <v>20.309961254843145</v>
       </c>
       <c r="I9">
         <v>0.6</v>
       </c>
       <c r="J9" s="5">
-        <v>1.3211999999999999</v>
+        <v>1.2861</v>
       </c>
       <c r="K9" s="5">
-        <v>1.7118</v>
+        <v>1.6632</v>
       </c>
       <c r="L9">
+        <f t="shared" si="5"/>
+        <v>0.77326839826839833</v>
+      </c>
+      <c r="M9">
         <f t="shared" si="3"/>
-        <v>0.77181913774973709</v>
+        <v>0.23149799999999998</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="2"/>
+        <v>0.1796256</v>
+      </c>
+      <c r="O9">
+        <f>ABS(M9-'Wind Tunnel Beta=29deg data'!B12)</f>
+        <v>1.149799999999998E-2</v>
+      </c>
+      <c r="P9">
+        <f>ABS(N9-'Wind Tunnel Beta=29deg data'!C12)</f>
+        <v>1.2874400000000008E-2</v>
       </c>
     </row>
-    <row r="10" spans="6:27" x14ac:dyDescent="0.35">
-      <c r="F10">
-        <f>H10*2*PI()*$Q$1/G10</f>
-        <v>9.666438934122441</v>
-      </c>
-      <c r="G10">
+    <row r="11" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I12" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
         <v>30</v>
       </c>
-      <c r="H10">
-        <f>G10/(I10*$Q$1)</f>
-        <v>21.631911395690921</v>
-      </c>
-      <c r="I10">
-        <v>0.65</v>
-      </c>
-      <c r="J10" s="5">
-        <v>1.0087999999999999</v>
-      </c>
-      <c r="K10" s="5">
-        <v>1.2592000000000001</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="3"/>
-        <v>0.80114358322744583</v>
+      <c r="K12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" t="s">
+        <v>0</v>
+      </c>
+      <c r="N12" t="s">
+        <v>7</v>
+      </c>
+      <c r="O12" t="s">
+        <v>32</v>
+      </c>
+      <c r="P12" t="s">
+        <v>33</v>
       </c>
     </row>
-    <row r="12" spans="6:27" x14ac:dyDescent="0.35">
-      <c r="F12" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" t="s">
-        <v>11</v>
+    <row r="13" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="F13">
+        <f t="shared" ref="F13" si="6">H13*2*PI()*$Q$1/G13</f>
+        <v>20.943951023931955</v>
+      </c>
+      <c r="G13">
+        <v>26</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ref="H13" si="7">G13/(I13*$Q$1)</f>
+        <v>40.61992250968629</v>
+      </c>
+      <c r="I13">
+        <v>0.3</v>
+      </c>
+      <c r="J13" s="5">
+        <v>3.8041999999999998</v>
+      </c>
+      <c r="K13" s="5">
+        <v>6.1909999999999998</v>
+      </c>
+      <c r="L13">
+        <f>J13/K13</f>
+        <v>0.61447262154740756</v>
+      </c>
+      <c r="M13">
+        <f>J13*POWER(I13,2)/2</f>
+        <v>0.17118899999999998</v>
+      </c>
+      <c r="N13">
+        <f>K13*POWER(I13,3)/2</f>
+        <v>8.35785E-2</v>
+      </c>
+      <c r="O13">
+        <f>ABS(M13-'Wind Tunnel Beta=19deg data'!B6)</f>
+        <v>1.6889999999999683E-3</v>
+      </c>
+      <c r="P13">
+        <f>ABS(N13-'Wind Tunnel Beta=19deg data'!C6)</f>
+        <v>1.0261500000000007E-2</v>
       </c>
     </row>
-    <row r="13" spans="6:27" x14ac:dyDescent="0.35">
-      <c r="F13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" t="s">
-        <v>9</v>
-      </c>
-      <c r="I13" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
-        <v>0</v>
-      </c>
-      <c r="K13" t="s">
-        <v>7</v>
-      </c>
-      <c r="L13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="6:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="6:27" x14ac:dyDescent="0.55000000000000004">
       <c r="F14">
-        <f t="shared" ref="F14" si="4">H14*2*PI()*$Q$1/G14</f>
-        <v>20.943951023931955</v>
+        <f t="shared" ref="F14:F19" si="8">H14*2*PI()*$Q$1/G14</f>
+        <v>17.951958020513104</v>
       </c>
       <c r="G14">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H14">
-        <f t="shared" ref="H14" si="5">G14/(I14*$Q$1)</f>
-        <v>46.869141357330335</v>
+        <f t="shared" ref="H14:H19" si="9">G14/(I14*$Q$1)</f>
+        <v>34.817076436873961</v>
       </c>
       <c r="I14">
-        <v>0.3</v>
+        <v>0.35</v>
       </c>
       <c r="J14" s="5">
-        <v>3.7530999999999999</v>
+        <v>2.4382000000000001</v>
       </c>
       <c r="K14" s="5">
-        <v>6.1067999999999998</v>
+        <v>3.6280000000000001</v>
       </c>
       <c r="L14">
         <f>J14/K14</f>
-        <v>0.61457719263771537</v>
+        <v>0.67205071664829108</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ref="M14:M19" si="10">J14*POWER(I14,2)/2</f>
+        <v>0.14933974999999999</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ref="N14:N19" si="11">K14*POWER(I14,3)/2</f>
+        <v>7.777524999999999E-2</v>
+      </c>
+      <c r="O14">
+        <f>ABS(M14-'Wind Tunnel Beta=19deg data'!B7)</f>
+        <v>1.6025000000000067E-4</v>
+      </c>
+      <c r="P14">
+        <f>ABS(N14-'Wind Tunnel Beta=19deg data'!C7)</f>
+        <v>1.2424750000000012E-2</v>
       </c>
     </row>
-    <row r="15" spans="6:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="6:27" x14ac:dyDescent="0.55000000000000004">
       <c r="F15">
-        <f t="shared" ref="F15:F21" si="6">H15*2*PI()*$Q$1/G15</f>
-        <v>17.951958020513107</v>
+        <f t="shared" si="8"/>
+        <v>15.707963267948967</v>
       </c>
       <c r="G15">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H15">
-        <f t="shared" ref="H15:H21" si="7">G15/(I15*$Q$1)</f>
-        <v>40.173549734854575</v>
+        <f t="shared" si="9"/>
+        <v>30.464941882264718</v>
       </c>
       <c r="I15">
-        <v>0.35</v>
+        <v>0.4</v>
       </c>
       <c r="J15" s="5">
-        <v>2.4028999999999998</v>
+        <v>1.6445000000000001</v>
       </c>
       <c r="K15" s="5">
-        <v>3.5200999999999998</v>
+        <v>2.2471999999999999</v>
       </c>
       <c r="L15">
         <f>J15/K15</f>
-        <v>0.68262265276554646</v>
+        <v>0.73179957280170882</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="10"/>
+        <v>0.13156000000000004</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="11"/>
+        <v>7.1910400000000013E-2</v>
+      </c>
+      <c r="O15">
+        <f>ABS(M15-'Wind Tunnel Beta=19deg data'!B8)</f>
+        <v>8.6000000000002741E-4</v>
+      </c>
+      <c r="P15">
+        <f>ABS(N15-'Wind Tunnel Beta=19deg data'!C8)</f>
+        <v>1.3529599999999989E-2</v>
       </c>
     </row>
-    <row r="16" spans="6:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="6:27" x14ac:dyDescent="0.55000000000000004">
       <c r="F16">
-        <f t="shared" si="6"/>
-        <v>15.707963267948966</v>
+        <f t="shared" si="8"/>
+        <v>13.962634015954636</v>
       </c>
       <c r="G16">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H16">
-        <f t="shared" si="7"/>
-        <v>35.151856017997751</v>
+        <f t="shared" si="9"/>
+        <v>27.07994833979086</v>
       </c>
       <c r="I16">
-        <v>0.4</v>
+        <v>0.45</v>
       </c>
       <c r="J16" s="5">
-        <v>1.5784</v>
+        <v>1.0670999999999999</v>
       </c>
       <c r="K16" s="5">
-        <v>2.1392000000000002</v>
+        <v>1.3714</v>
       </c>
       <c r="L16">
         <f>J16/K16</f>
-        <v>0.73784592370979796</v>
+        <v>0.7781099606241797</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="10"/>
+        <v>0.108043875</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="11"/>
+        <v>6.2484412500000003E-2</v>
+      </c>
+      <c r="O16">
+        <f>ABS(M16-'Wind Tunnel Beta=19deg data'!B9)</f>
+        <v>3.8561250000000019E-3</v>
+      </c>
+      <c r="P16">
+        <f>ABS(N16-'Wind Tunnel Beta=19deg data'!C9)</f>
+        <v>1.6705587499999994E-2</v>
       </c>
     </row>
-    <row r="17" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="6:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F17">
-        <f t="shared" si="6"/>
-        <v>13.962634015954638</v>
+        <f t="shared" si="8"/>
+        <v>12.566370614359174</v>
       </c>
       <c r="G17">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H17">
-        <f t="shared" si="7"/>
-        <v>31.246094238220223</v>
+        <f t="shared" si="9"/>
+        <v>24.371953505811774</v>
       </c>
       <c r="I17">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="J17" s="5">
-        <v>1.0024999999999999</v>
+        <v>0.69347999999999999</v>
       </c>
       <c r="K17" s="5">
-        <v>1.2854000000000001</v>
+        <v>0.86065999999999998</v>
       </c>
       <c r="L17">
-        <f>J17/K17</f>
-        <v>0.77991286758985523</v>
+        <f t="shared" ref="L17:L19" si="12">J17/K17</f>
+        <v>0.80575372388631983</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="10"/>
+        <v>8.6684999999999998E-2</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="11"/>
+        <v>5.3791249999999999E-2</v>
+      </c>
+      <c r="O17">
+        <f>ABS(M17-'Wind Tunnel Beta=19deg data'!B10)</f>
+        <v>2.6650000000000007E-3</v>
+      </c>
+      <c r="P17">
+        <f>ABS(N17-'Wind Tunnel Beta=19deg data'!C10)</f>
+        <v>1.8028749999999996E-2</v>
       </c>
     </row>
-    <row r="18" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F18">
-        <f t="shared" si="6"/>
-        <v>12.566370614359171</v>
+        <f t="shared" si="8"/>
+        <v>11.423973285781063</v>
       </c>
       <c r="G18">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H18">
-        <f t="shared" si="7"/>
-        <v>28.121484814398201</v>
+        <f t="shared" si="9"/>
+        <v>22.156321368919791</v>
       </c>
       <c r="I18">
-        <v>0.5</v>
+        <v>0.55000000000000004</v>
       </c>
       <c r="J18" s="5">
-        <v>0.65625</v>
+        <v>0.45036999999999999</v>
       </c>
       <c r="K18" s="5">
-        <v>0.81101999999999996</v>
+        <v>0.54393999999999998</v>
       </c>
       <c r="L18">
-        <f t="shared" ref="L18:L21" si="8">J18/K18</f>
-        <v>0.80916623511134134</v>
+        <f t="shared" si="12"/>
+        <v>0.82797735044306364</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="10"/>
+        <v>6.8118462500000004E-2</v>
+      </c>
+      <c r="N18">
+        <f t="shared" si="11"/>
+        <v>4.5249008750000014E-2</v>
+      </c>
+      <c r="O18">
+        <f>ABS(M18-'Wind Tunnel Beta=19deg data'!B11)</f>
+        <v>3.7015374999999906E-3</v>
+      </c>
+      <c r="P18">
+        <f>ABS(N18-'Wind Tunnel Beta=19deg data'!C11)</f>
+        <v>1.9220991249999986E-2</v>
       </c>
     </row>
-    <row r="19" spans="6:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F19">
-        <f t="shared" si="6"/>
-        <v>11.423973285781065</v>
+        <f t="shared" si="8"/>
+        <v>10.471975511965978</v>
       </c>
       <c r="G19">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H19">
-        <f t="shared" si="7"/>
-        <v>25.564986194907451</v>
+        <f t="shared" si="9"/>
+        <v>20.309961254843145</v>
       </c>
       <c r="I19">
-        <v>0.55000000000000004</v>
+        <v>0.6</v>
       </c>
       <c r="J19" s="5">
-        <v>0.41277000000000003</v>
+        <v>0.25535000000000002</v>
       </c>
       <c r="K19" s="5">
-        <v>0.50260000000000005</v>
+        <v>0.31189</v>
       </c>
       <c r="L19">
-        <f t="shared" si="8"/>
-        <v>0.82126939912455232</v>
-      </c>
-    </row>
-    <row r="20" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F20">
-        <f t="shared" si="6"/>
-        <v>10.471975511965978</v>
-      </c>
-      <c r="G20">
-        <v>30</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="7"/>
-        <v>23.434570678665168</v>
-      </c>
-      <c r="I20">
-        <v>0.6</v>
-      </c>
-      <c r="J20" s="5">
-        <v>0.24399000000000001</v>
-      </c>
-      <c r="K20" s="5">
-        <v>0.29807</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="8"/>
-        <v>0.81856610863220047</v>
-      </c>
-    </row>
-    <row r="21" spans="6:12" x14ac:dyDescent="0.35">
-      <c r="F21">
-        <f t="shared" si="6"/>
-        <v>9.666438934122441</v>
-      </c>
-      <c r="G21">
-        <v>30</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="7"/>
-        <v>21.631911395690921</v>
-      </c>
-      <c r="I21">
-        <v>0.65</v>
-      </c>
-      <c r="J21" s="5">
-        <v>0.10974</v>
-      </c>
-      <c r="K21" s="5">
-        <v>0.14926</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="8"/>
-        <v>0.73522712046094063</v>
+        <f t="shared" si="12"/>
+        <v>0.81871813780499547</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="10"/>
+        <v>4.5963000000000004E-2</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="11"/>
+        <v>3.3684119999999998E-2</v>
+      </c>
+      <c r="O19">
+        <f>ABS(M19-'Wind Tunnel Beta=19deg data'!B12)</f>
+        <v>4.0369999999999989E-3</v>
+      </c>
+      <c r="P19">
+        <f>ABS(N19-'Wind Tunnel Beta=19deg data'!C12)</f>
+        <v>2.4515880000000004E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor objectives and repair logic; improve efficiency objective description; update error handling in MTSOL_call; remove unused code and streamline directory management in X22A_validator.
</commit_message>
<xml_diff>
--- a/Validation/WindTunnelData.xlsx
+++ b/Validation/WindTunnelData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b266c95a83fbf4bb/Documenten/TU Delft Aerospace Engineering/Msc2/AE5222 - Thesis/Software/Conceptual-Investigation-of-Alternative-Electric-Ducted-Fan-Architectures/Validation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1585" documentId="8_{E7BF6703-466F-4498-AEEA-FFB8403C4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F76418B-819D-4D34-B006-8FC6AE60D8D6}"/>
+  <xr:revisionPtr revIDLastSave="1621" documentId="8_{E7BF6703-466F-4498-AEEA-FFB8403C4F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08067C1C-07CF-490C-9726-36A8D6D61930}"/>
   <bookViews>
-    <workbookView xWindow="14325" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="3" xr2:uid="{6111FCF9-37F3-4199-9E4E-EEB7F0803D9A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" firstSheet="2" activeTab="3" xr2:uid="{6111FCF9-37F3-4199-9E4E-EEB7F0803D9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Wind Tunnel Beta=29deg data" sheetId="16" r:id="rId1"/>
@@ -269,10 +269,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -861,16 +861,16 @@
                   <c:v>6.3601000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.5932000000000004</c:v>
+                  <c:v>4.5551000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.19</c:v>
+                  <c:v>3.1610999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.2608999999999999</c:v>
+                  <c:v>2.2736000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6632</c:v>
+                  <c:v>1.6722999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1622,25 +1622,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>6.1909999999999998</c:v>
+                  <c:v>6.2149999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6280000000000001</c:v>
+                  <c:v>3.6671999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2471999999999999</c:v>
+                  <c:v>2.2458</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3714</c:v>
+                  <c:v>1.3711</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.86065999999999998</c:v>
+                  <c:v>0.86234</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.54393999999999998</c:v>
+                  <c:v>0.54491999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.31189</c:v>
+                  <c:v>0.31276999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2395,22 +2395,22 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.20028749999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.32695200000000008</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.30411450000000001</c:v>
+                  <c:v>0.26620650000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.27928750000000002</c:v>
+                  <c:v>0.27700000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.253237875</c:v>
+                  <c:v>0.25444787500000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.23149799999999998</c:v>
+                  <c:v>0.23257800000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3095,25 +3095,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.17118899999999998</c:v>
+                  <c:v>0.17098649999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14933974999999999</c:v>
+                  <c:v>0.15189387499999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.13156000000000004</c:v>
+                  <c:v>0.13146400000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.108043875</c:v>
+                  <c:v>0.108003375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.6684999999999998E-2</c:v>
+                  <c:v>8.6804999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.8118462500000004E-2</c:v>
+                  <c:v>6.8216775000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.5963000000000004E-2</c:v>
+                  <c:v>4.60782E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7507,24 +7507,27 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'test results - with crash handl'!$J$4:$J$9</c:f>
+              <c:f>'test results - with crash handl'!$J$3:$J$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="1">
+                  <c:v>3.27</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>4.0869</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.0036</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2343000000000002</c:v>
+                  <c:v>2.6292</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6742999999999999</c:v>
+                  <c:v>2.2160000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2861</c:v>
+                  <c:v>1.6822999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2921</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8426,25 +8429,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.8041999999999998</c:v>
+                  <c:v>3.7997000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4382000000000001</c:v>
+                  <c:v>2.4799000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6445000000000001</c:v>
+                  <c:v>1.6433</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0670999999999999</c:v>
+                  <c:v>1.0667</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.69347999999999999</c:v>
+                  <c:v>0.69443999999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.45036999999999999</c:v>
+                  <c:v>0.45101999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25535000000000002</c:v>
+                  <c:v>0.25599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16982,24 +16985,24 @@
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -17007,7 +17010,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -17039,7 +17042,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.3</v>
       </c>
@@ -17078,7 +17081,7 @@
         <v>0.74074074074074081</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.35</v>
       </c>
@@ -17117,7 +17120,7 @@
         <v>0.46647230320699723</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.4</v>
       </c>
@@ -17156,7 +17159,7 @@
         <v>0.31249999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.45</v>
       </c>
@@ -17195,7 +17198,7 @@
         <v>0.21947873799725648</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.5</v>
       </c>
@@ -17234,7 +17237,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.55000000000000004</v>
       </c>
@@ -17273,7 +17276,7 @@
         <v>0.12021036814425241</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.6</v>
       </c>
@@ -17334,24 +17337,24 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -17359,7 +17362,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -17391,7 +17394,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.3</v>
       </c>
@@ -17430,7 +17433,7 @@
         <v>0.74074074074074081</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.35</v>
       </c>
@@ -17469,7 +17472,7 @@
         <v>0.46647230320699723</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.4</v>
       </c>
@@ -17508,7 +17511,7 @@
         <v>0.31249999999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.45</v>
       </c>
@@ -17547,7 +17550,7 @@
         <v>0.21947873799725648</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.5</v>
       </c>
@@ -17586,7 +17589,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.55000000000000004</v>
       </c>
@@ -17625,7 +17628,7 @@
         <v>0.12021036814425241</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.6</v>
       </c>
@@ -17686,12 +17689,12 @@
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="15" max="15" width="11.62890625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F1" t="s">
         <v>2</v>
       </c>
@@ -17712,7 +17715,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F2" t="s">
         <v>3</v>
       </c>
@@ -17739,7 +17742,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F3">
         <f>H3*2*PI()*$P$1/G3</f>
         <v>20.943951023931955</v>
@@ -17763,7 +17766,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F4">
         <f t="shared" ref="F4:F9" si="0">H4*2*PI()*$P$1/G4</f>
         <v>17.951958020513104</v>
@@ -17787,7 +17790,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F5">
         <f t="shared" si="0"/>
         <v>15.707963267948966</v>
@@ -17813,7 +17816,7 @@
         <v>0.66311381150987769</v>
       </c>
     </row>
-    <row r="6" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F6">
         <f t="shared" si="0"/>
         <v>13.962634015954636</v>
@@ -17837,7 +17840,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="7" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F7">
         <f t="shared" si="0"/>
         <v>12.566370614359172</v>
@@ -17863,7 +17866,7 @@
         <v>0.7222979181849869</v>
       </c>
     </row>
-    <row r="8" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F8">
         <f t="shared" si="0"/>
         <v>11.423973285781065</v>
@@ -17889,7 +17892,7 @@
         <v>0.73735942999399084</v>
       </c>
     </row>
-    <row r="9" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F9">
         <f t="shared" si="0"/>
         <v>10.471975511965978</v>
@@ -17918,37 +17921,37 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="6:41" ht="65.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="AG10" s="7" t="s">
+    <row r="10" spans="6:41" ht="65.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AG10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="AH10" s="7"/>
-      <c r="AI10" s="7"/>
-      <c r="AJ10" s="7"/>
-      <c r="AK10" s="7"/>
-      <c r="AL10" s="7"/>
-      <c r="AM10" s="7"/>
-      <c r="AN10" s="7"/>
-      <c r="AO10" s="7"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
+      <c r="AJ10" s="8"/>
+      <c r="AK10" s="8"/>
+      <c r="AL10" s="8"/>
+      <c r="AM10" s="8"/>
+      <c r="AN10" s="8"/>
+      <c r="AO10" s="8"/>
     </row>
-    <row r="11" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F11" t="s">
         <v>2</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
-      <c r="AG11" s="7"/>
-      <c r="AH11" s="7"/>
-      <c r="AI11" s="7"/>
-      <c r="AJ11" s="7"/>
-      <c r="AK11" s="7"/>
-      <c r="AL11" s="7"/>
-      <c r="AM11" s="7"/>
-      <c r="AN11" s="7"/>
-      <c r="AO11" s="7"/>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
+      <c r="AI11" s="8"/>
+      <c r="AJ11" s="8"/>
+      <c r="AK11" s="8"/>
+      <c r="AL11" s="8"/>
+      <c r="AM11" s="8"/>
+      <c r="AN11" s="8"/>
+      <c r="AO11" s="8"/>
     </row>
-    <row r="12" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F12" t="s">
         <v>3</v>
       </c>
@@ -17971,7 +17974,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F13">
         <f>H13*2*PI()*$P$1/G13</f>
         <v>20.943951023931955</v>
@@ -17991,7 +17994,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F14">
         <f t="shared" ref="F14:F19" si="3">H14*2*PI()*$P$1/G14</f>
         <v>17.951958020513104</v>
@@ -18017,7 +18020,7 @@
         <v>0.68237501065855666</v>
       </c>
     </row>
-    <row r="15" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F15">
         <f t="shared" si="3"/>
         <v>15.707963267948966</v>
@@ -18043,7 +18046,7 @@
         <v>0.73950214916631241</v>
       </c>
     </row>
-    <row r="16" spans="6:41" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="6:41" x14ac:dyDescent="0.35">
       <c r="F16">
         <f t="shared" si="3"/>
         <v>13.962634015954636</v>
@@ -18069,7 +18072,7 @@
         <v>0.783448275862069</v>
       </c>
     </row>
-    <row r="17" spans="6:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F17">
         <f t="shared" si="3"/>
         <v>12.566370614359172</v>
@@ -18095,7 +18098,7 @@
         <v>0.8144490579683038</v>
       </c>
     </row>
-    <row r="18" spans="6:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F18">
         <f t="shared" si="3"/>
         <v>11.423973285781065</v>
@@ -18121,7 +18124,7 @@
         <v>0.82430531487635328</v>
       </c>
     </row>
-    <row r="19" spans="6:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="6:12" x14ac:dyDescent="0.35">
       <c r="F19">
         <f t="shared" si="3"/>
         <v>10.471975511965978</v>
@@ -18163,16 +18166,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC9A3C9B-DBC3-40D2-A144-241D094FABD6}">
   <dimension ref="F1:AA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="158" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J10" sqref="I10:J10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="158" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="16" max="16" width="11.62890625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F1" t="s">
         <v>2</v>
       </c>
@@ -18193,7 +18196,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F2" t="s">
         <v>3</v>
       </c>
@@ -18232,7 +18235,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="6:27" ht="14.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="6:27" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F3">
         <f t="shared" ref="F3:F5" si="0">H3*2*PI()*$Q$1/G3</f>
         <v>20.943951023931955</v>
@@ -18274,7 +18277,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="6:27" ht="14.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="6:27" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F4">
         <f t="shared" si="0"/>
         <v>17.951958020513104</v>
@@ -18289,15 +18292,17 @@
       <c r="I4">
         <v>0.35</v>
       </c>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
+      <c r="J4" s="7">
+        <v>3.27</v>
+      </c>
+      <c r="K4" s="7"/>
       <c r="L4" t="e">
         <f>J4/K4</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M4">
         <f>J4*POWER(I4,2)/2</f>
-        <v>0</v>
+        <v>0.20028749999999998</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N9" si="2">K4*POWER(I4,3)/2</f>
@@ -18305,7 +18310,7 @@
       </c>
       <c r="O4">
         <f>ABS(M4-'Wind Tunnel Beta=29deg data'!B7)</f>
-        <v>0.35</v>
+        <v>0.1497125</v>
       </c>
       <c r="P4">
         <f>ABS(N4-'Wind Tunnel Beta=29deg data'!C7)</f>
@@ -18316,7 +18321,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F5">
         <f t="shared" si="0"/>
         <v>15.707963267948967</v>
@@ -18342,7 +18347,7 @@
         <v>0.64258423609691673</v>
       </c>
       <c r="M5">
-        <f t="shared" ref="M4:M9" si="3">J5*POWER(I5,2)/2</f>
+        <f t="shared" ref="M5:M9" si="3">J5*POWER(I5,2)/2</f>
         <v>0.32695200000000008</v>
       </c>
       <c r="N5">
@@ -18362,7 +18367,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F6">
         <f>H6*2*PI()*$Q$1/G6</f>
         <v>13.962634015954636</v>
@@ -18378,33 +18383,33 @@
         <v>0.45</v>
       </c>
       <c r="J6" s="5">
-        <v>3.0036</v>
+        <v>2.6292</v>
       </c>
       <c r="K6" s="5">
-        <v>4.5932000000000004</v>
+        <v>4.5551000000000004</v>
       </c>
       <c r="L6">
         <f>J6/K6</f>
-        <v>0.65392319080379691</v>
+        <v>0.57719918333296738</v>
       </c>
       <c r="M6">
         <f t="shared" si="3"/>
-        <v>0.30411450000000001</v>
+        <v>0.26620650000000001</v>
       </c>
       <c r="N6">
         <f t="shared" si="2"/>
-        <v>0.20927767500000005</v>
+        <v>0.20754174375000004</v>
       </c>
       <c r="O6">
         <f>ABS(M6-'Wind Tunnel Beta=29deg data'!B9)</f>
-        <v>8.1145000000000245E-3</v>
+        <v>2.9793499999999973E-2</v>
       </c>
       <c r="P6">
         <f>ABS(N6-'Wind Tunnel Beta=29deg data'!C9)</f>
-        <v>1.2422324999999956E-2</v>
+        <v>1.4158256249999973E-2</v>
       </c>
     </row>
-    <row r="7" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F7">
         <f t="shared" ref="F7:F8" si="4">H7*2*PI()*$Q$1/G7</f>
         <v>12.566370614359174</v>
@@ -18420,33 +18425,33 @@
         <v>0.5</v>
       </c>
       <c r="J7" s="5">
-        <v>2.2343000000000002</v>
+        <v>2.2160000000000002</v>
       </c>
       <c r="K7" s="5">
-        <v>3.19</v>
+        <v>3.1610999999999998</v>
       </c>
       <c r="L7">
         <f t="shared" ref="L7:L9" si="5">J7/K7</f>
-        <v>0.70040752351097191</v>
+        <v>0.70102179621018013</v>
       </c>
       <c r="M7">
         <f t="shared" si="3"/>
-        <v>0.27928750000000002</v>
+        <v>0.27700000000000002</v>
       </c>
       <c r="N7">
         <f t="shared" si="2"/>
-        <v>0.199375</v>
+        <v>0.19756874999999999</v>
       </c>
       <c r="O7">
         <f>ABS(M7-'Wind Tunnel Beta=29deg data'!B10)</f>
-        <v>9.2875000000000041E-3</v>
+        <v>7.0000000000000062E-3</v>
       </c>
       <c r="P7">
         <f>ABS(N7-'Wind Tunnel Beta=29deg data'!C10)</f>
-        <v>1.5025000000000011E-2</v>
+        <v>1.683125000000002E-2</v>
       </c>
     </row>
-    <row r="8" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F8">
         <f t="shared" si="4"/>
         <v>11.423973285781063</v>
@@ -18462,33 +18467,33 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="J8" s="5">
-        <v>1.6742999999999999</v>
+        <v>1.6822999999999999</v>
       </c>
       <c r="K8" s="5">
-        <v>2.2608999999999999</v>
+        <v>2.2736000000000001</v>
       </c>
       <c r="L8">
         <f t="shared" si="5"/>
-        <v>0.74054580034499529</v>
+        <v>0.73992786769880359</v>
       </c>
       <c r="M8">
         <f t="shared" si="3"/>
-        <v>0.253237875</v>
+        <v>0.25444787500000005</v>
       </c>
       <c r="N8">
         <f t="shared" si="2"/>
-        <v>0.18807861875000004</v>
+        <v>0.18913510000000006</v>
       </c>
       <c r="O8">
         <f>ABS(M8-'Wind Tunnel Beta=29deg data'!B11)</f>
-        <v>7.2378750000000047E-3</v>
+        <v>8.4478750000000491E-3</v>
       </c>
       <c r="P8">
         <f>ABS(N8-'Wind Tunnel Beta=29deg data'!C11)</f>
-        <v>1.592138124999995E-2</v>
+        <v>1.4864899999999931E-2</v>
       </c>
     </row>
-    <row r="9" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F9">
         <f>H9*2*PI()*$Q$1/G9</f>
         <v>10.471975511965978</v>
@@ -18504,33 +18509,33 @@
         <v>0.6</v>
       </c>
       <c r="J9" s="5">
-        <v>1.2861</v>
+        <v>1.2921</v>
       </c>
       <c r="K9" s="5">
-        <v>1.6632</v>
+        <v>1.6722999999999999</v>
       </c>
       <c r="L9">
         <f t="shared" si="5"/>
-        <v>0.77326839826839833</v>
+        <v>0.77264844824493217</v>
       </c>
       <c r="M9">
         <f t="shared" si="3"/>
-        <v>0.23149799999999998</v>
+        <v>0.23257800000000001</v>
       </c>
       <c r="N9">
         <f t="shared" si="2"/>
-        <v>0.1796256</v>
+        <v>0.18060839999999997</v>
       </c>
       <c r="O9">
         <f>ABS(M9-'Wind Tunnel Beta=29deg data'!B12)</f>
-        <v>1.149799999999998E-2</v>
+        <v>1.2578000000000006E-2</v>
       </c>
       <c r="P9">
         <f>ABS(N9-'Wind Tunnel Beta=29deg data'!C12)</f>
-        <v>1.2874400000000008E-2</v>
+        <v>1.189160000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F11" t="s">
         <v>2</v>
       </c>
@@ -18538,7 +18543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F12" t="s">
         <v>3</v>
       </c>
@@ -18573,7 +18578,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F13">
         <f t="shared" ref="F13" si="6">H13*2*PI()*$Q$1/G13</f>
         <v>20.943951023931955</v>
@@ -18589,33 +18594,33 @@
         <v>0.3</v>
       </c>
       <c r="J13" s="5">
-        <v>3.8041999999999998</v>
+        <v>3.7997000000000001</v>
       </c>
       <c r="K13" s="5">
-        <v>6.1909999999999998</v>
+        <v>6.2149999999999999</v>
       </c>
       <c r="L13">
         <f>J13/K13</f>
-        <v>0.61447262154740756</v>
+        <v>0.61137570394207563</v>
       </c>
       <c r="M13">
         <f>J13*POWER(I13,2)/2</f>
-        <v>0.17118899999999998</v>
+        <v>0.17098649999999999</v>
       </c>
       <c r="N13">
         <f>K13*POWER(I13,3)/2</f>
-        <v>8.35785E-2</v>
+        <v>8.3902499999999991E-2</v>
       </c>
       <c r="O13">
         <f>ABS(M13-'Wind Tunnel Beta=19deg data'!B6)</f>
-        <v>1.6889999999999683E-3</v>
+        <v>1.486499999999974E-3</v>
       </c>
       <c r="P13">
         <f>ABS(N13-'Wind Tunnel Beta=19deg data'!C6)</f>
-        <v>1.0261500000000007E-2</v>
+        <v>9.9375000000000158E-3</v>
       </c>
     </row>
-    <row r="14" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F14">
         <f t="shared" ref="F14:F19" si="8">H14*2*PI()*$Q$1/G14</f>
         <v>17.951958020513104</v>
@@ -18631,33 +18636,33 @@
         <v>0.35</v>
       </c>
       <c r="J14" s="5">
-        <v>2.4382000000000001</v>
+        <v>2.4799000000000002</v>
       </c>
       <c r="K14" s="5">
-        <v>3.6280000000000001</v>
+        <v>3.6671999999999998</v>
       </c>
       <c r="L14">
         <f>J14/K14</f>
-        <v>0.67205071664829108</v>
+        <v>0.67623800174520077</v>
       </c>
       <c r="M14">
         <f t="shared" ref="M14:M19" si="10">J14*POWER(I14,2)/2</f>
-        <v>0.14933974999999999</v>
+        <v>0.15189387499999998</v>
       </c>
       <c r="N14">
         <f t="shared" ref="N14:N19" si="11">K14*POWER(I14,3)/2</f>
-        <v>7.777524999999999E-2</v>
+        <v>7.861559999999998E-2</v>
       </c>
       <c r="O14">
         <f>ABS(M14-'Wind Tunnel Beta=19deg data'!B7)</f>
-        <v>1.6025000000000067E-4</v>
+        <v>2.3938749999999898E-3</v>
       </c>
       <c r="P14">
         <f>ABS(N14-'Wind Tunnel Beta=19deg data'!C7)</f>
-        <v>1.2424750000000012E-2</v>
+        <v>1.1584400000000022E-2</v>
       </c>
     </row>
-    <row r="15" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F15">
         <f t="shared" si="8"/>
         <v>15.707963267948967</v>
@@ -18673,33 +18678,33 @@
         <v>0.4</v>
       </c>
       <c r="J15" s="5">
-        <v>1.6445000000000001</v>
+        <v>1.6433</v>
       </c>
       <c r="K15" s="5">
-        <v>2.2471999999999999</v>
+        <v>2.2458</v>
       </c>
       <c r="L15">
         <f>J15/K15</f>
-        <v>0.73179957280170882</v>
+        <v>0.73172143556861691</v>
       </c>
       <c r="M15">
         <f t="shared" si="10"/>
-        <v>0.13156000000000004</v>
+        <v>0.13146400000000003</v>
       </c>
       <c r="N15">
         <f t="shared" si="11"/>
-        <v>7.1910400000000013E-2</v>
+        <v>7.1865600000000016E-2</v>
       </c>
       <c r="O15">
         <f>ABS(M15-'Wind Tunnel Beta=19deg data'!B8)</f>
-        <v>8.6000000000002741E-4</v>
+        <v>7.6400000000001467E-4</v>
       </c>
       <c r="P15">
         <f>ABS(N15-'Wind Tunnel Beta=19deg data'!C8)</f>
-        <v>1.3529599999999989E-2</v>
+        <v>1.3574399999999986E-2</v>
       </c>
     </row>
-    <row r="16" spans="6:27" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="6:27" x14ac:dyDescent="0.35">
       <c r="F16">
         <f t="shared" si="8"/>
         <v>13.962634015954636</v>
@@ -18715,33 +18720,33 @@
         <v>0.45</v>
       </c>
       <c r="J16" s="5">
-        <v>1.0670999999999999</v>
+        <v>1.0667</v>
       </c>
       <c r="K16" s="5">
-        <v>1.3714</v>
+        <v>1.3711</v>
       </c>
       <c r="L16">
         <f>J16/K16</f>
-        <v>0.7781099606241797</v>
+        <v>0.7779884764058056</v>
       </c>
       <c r="M16">
         <f t="shared" si="10"/>
-        <v>0.108043875</v>
+        <v>0.108003375</v>
       </c>
       <c r="N16">
         <f t="shared" si="11"/>
-        <v>6.2484412500000003E-2</v>
+        <v>6.2470743750000009E-2</v>
       </c>
       <c r="O16">
         <f>ABS(M16-'Wind Tunnel Beta=19deg data'!B9)</f>
-        <v>3.8561250000000019E-3</v>
+        <v>3.8966250000000008E-3</v>
       </c>
       <c r="P16">
         <f>ABS(N16-'Wind Tunnel Beta=19deg data'!C9)</f>
-        <v>1.6705587499999994E-2</v>
+        <v>1.6719256249999988E-2</v>
       </c>
     </row>
-    <row r="17" spans="6:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="6:16" x14ac:dyDescent="0.35">
       <c r="F17">
         <f t="shared" si="8"/>
         <v>12.566370614359174</v>
@@ -18757,33 +18762,33 @@
         <v>0.5</v>
       </c>
       <c r="J17" s="5">
-        <v>0.69347999999999999</v>
+        <v>0.69443999999999995</v>
       </c>
       <c r="K17" s="5">
-        <v>0.86065999999999998</v>
+        <v>0.86234</v>
       </c>
       <c r="L17">
         <f t="shared" ref="L17:L19" si="12">J17/K17</f>
-        <v>0.80575372388631983</v>
+        <v>0.80529721455574366</v>
       </c>
       <c r="M17">
         <f t="shared" si="10"/>
-        <v>8.6684999999999998E-2</v>
+        <v>8.6804999999999993E-2</v>
       </c>
       <c r="N17">
         <f t="shared" si="11"/>
-        <v>5.3791249999999999E-2</v>
+        <v>5.389625E-2</v>
       </c>
       <c r="O17">
         <f>ABS(M17-'Wind Tunnel Beta=19deg data'!B10)</f>
-        <v>2.6650000000000007E-3</v>
+        <v>2.5450000000000056E-3</v>
       </c>
       <c r="P17">
         <f>ABS(N17-'Wind Tunnel Beta=19deg data'!C10)</f>
-        <v>1.8028749999999996E-2</v>
+        <v>1.7923749999999995E-2</v>
       </c>
     </row>
-    <row r="18" spans="6:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="6:16" x14ac:dyDescent="0.35">
       <c r="F18">
         <f t="shared" si="8"/>
         <v>11.423973285781063</v>
@@ -18799,33 +18804,33 @@
         <v>0.55000000000000004</v>
       </c>
       <c r="J18" s="5">
-        <v>0.45036999999999999</v>
+        <v>0.45101999999999998</v>
       </c>
       <c r="K18" s="5">
-        <v>0.54393999999999998</v>
+        <v>0.54491999999999996</v>
       </c>
       <c r="L18">
         <f t="shared" si="12"/>
-        <v>0.82797735044306364</v>
+        <v>0.82768112750495493</v>
       </c>
       <c r="M18">
         <f t="shared" si="10"/>
-        <v>6.8118462500000004E-2</v>
+        <v>6.8216775000000007E-2</v>
       </c>
       <c r="N18">
         <f t="shared" si="11"/>
-        <v>4.5249008750000014E-2</v>
+        <v>4.5330532500000013E-2</v>
       </c>
       <c r="O18">
         <f>ABS(M18-'Wind Tunnel Beta=19deg data'!B11)</f>
-        <v>3.7015374999999906E-3</v>
+        <v>3.6032249999999877E-3</v>
       </c>
       <c r="P18">
         <f>ABS(N18-'Wind Tunnel Beta=19deg data'!C11)</f>
-        <v>1.9220991249999986E-2</v>
+        <v>1.9139467499999986E-2</v>
       </c>
     </row>
-    <row r="19" spans="6:16" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="6:16" x14ac:dyDescent="0.35">
       <c r="F19">
         <f t="shared" si="8"/>
         <v>10.471975511965978</v>
@@ -18841,30 +18846,30 @@
         <v>0.6</v>
       </c>
       <c r="J19" s="5">
-        <v>0.25535000000000002</v>
+        <v>0.25599</v>
       </c>
       <c r="K19" s="5">
-        <v>0.31189</v>
+        <v>0.31276999999999999</v>
       </c>
       <c r="L19">
         <f t="shared" si="12"/>
-        <v>0.81871813780499547</v>
+        <v>0.81846084982575051</v>
       </c>
       <c r="M19">
         <f t="shared" si="10"/>
-        <v>4.5963000000000004E-2</v>
+        <v>4.60782E-2</v>
       </c>
       <c r="N19">
         <f t="shared" si="11"/>
-        <v>3.3684119999999998E-2</v>
+        <v>3.3779159999999996E-2</v>
       </c>
       <c r="O19">
         <f>ABS(M19-'Wind Tunnel Beta=19deg data'!B12)</f>
-        <v>4.0369999999999989E-3</v>
+        <v>3.9218000000000031E-3</v>
       </c>
       <c r="P19">
         <f>ABS(N19-'Wind Tunnel Beta=19deg data'!C12)</f>
-        <v>2.4515880000000004E-2</v>
+        <v>2.4420840000000006E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>